<commit_message>
dictionaries are placed in separate files and partially edited
</commit_message>
<xml_diff>
--- a/словарьТЗ.xlsx
+++ b/словарьТЗ.xlsx
@@ -5,17 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shapovv/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shapovv/PycharmProjects/Radost/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E6A5006-BB12-EC4F-9040-E1D70C054A36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D2ACFAA-E34F-7A44-9FC0-90E6A99B09CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="14560" windowHeight="16840" xr2:uid="{5429B6A6-3AB4-3F43-B880-B81809A67136}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="18860" windowHeight="16840" xr2:uid="{5429B6A6-3AB4-3F43-B880-B81809A67136}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -233,21 +233,9 @@
     <t>Приступим к созданию вашего технического задания. Сейчас мы поэтапно пройдём по всем пунктам, начиная с титульного листа и заканчивая списком литературы. Следуйте дальнейшим указаниям и подсказкам. В любом месте вы можете остановиться и отправить ответ позднее, а если захотите закончить и получить документ с не до конца введёнными данными, введите /stop. Если вы хотите пропустить любой шаг, необходимо отправить в ответи любой символ, тогда вы сможете заполнить этот раздел самостоятельно в итоговом документе.</t>
   </si>
   <si>
-    <t>Переходим к заполнению раздела "Введение".\n\nНапишите краткую характеристику области применения программы, например "«Генератор документации ‘‘Радость Научника’’» — прикладная программа, разрабатываемая с целью облегчения формирования и оформления документации."</t>
-  </si>
-  <si>
-    <t>Переходим к разделу "Назначение разработки".\n\nВведите функциональное назначение</t>
-  </si>
-  <si>
     <t>Введите эксплуатационное назначение</t>
   </si>
   <si>
-    <t>Переходим к разделу "Основания для разработки".\n\nВведите основания для разработки, это может быть, например, указ ректора или учебный план</t>
-  </si>
-  <si>
-    <t>Переходим к разделу "Требования к программе".\n\nВведите требования к составу выполняемых функций</t>
-  </si>
-  <si>
     <t>Введите требования к организации входных данных</t>
   </si>
   <si>
@@ -269,18 +257,9 @@
     <t>Введите требования к численности и квалификации персонала</t>
   </si>
   <si>
-    <t>Переходим к разделу "Требования к документации".\n\nВведите специальные требования к программной документации</t>
-  </si>
-  <si>
     <t>Опишите предполагаемую потребность</t>
   </si>
   <si>
-    <t>Следующий раздел "Техникоэкономические показатели"\n\nОпишите ориентировочную экономическую эффективность</t>
-  </si>
-  <si>
-    <t>Заполним сравнительную таблицу с аналогами. По умолчанию она имеет вид таблицы с тремя аналогами и пятью сравнительными характеристиками. В итоговом файле вы сможете изменить их количество.\n\nВведите название первого аналога</t>
-  </si>
-  <si>
     <t>Введите название второго аналога</t>
   </si>
   <si>
@@ -302,15 +281,6 @@
     <t>Введите пятую сравнительную характеристику</t>
   </si>
   <si>
-    <t>Седующий раздел "Порядок контроля и приемки".\n\nВведите виды испытаний</t>
-  </si>
-  <si>
-    <t>Заключительный раздел "Список использованных источников".\n\nПо умолчанию в него включены 10 основных ГОСТ-ов, по которым оформляется техническое задание. Чтобы добавить свои источники, введите их через перевод строки в одном сообщении</t>
-  </si>
-  <si>
-    <t>Сначала заполним титульный лист.\n\nВведите полное название ВУЗа, например "Национальный исследовательский университет Высшая Школа Экономики"</t>
-  </si>
-  <si>
     <t>Введите название работы, например «Генератор документации "Радость Научника"»</t>
   </si>
   <si>
@@ -318,6 +288,36 @@
   </si>
   <si>
     <t>Введите год</t>
+  </si>
+  <si>
+    <t>&lt;b&gt;Сначала заполним титульный лист.&lt;/b&gt;\n\nВведите полное название ВУЗа, например "Национальный исследовательский университет Высшая Школа Экономики"</t>
+  </si>
+  <si>
+    <t>&lt;b&gt;Переходим к заполнению раздела "Введение".&lt;/b&gt;\n\nНапишите краткую характеристику области применения программы, например "«Генератор документации ‘‘Радость Научника’’» — прикладная программа, разрабатываемая с целью облегчения формирования и оформления документации."</t>
+  </si>
+  <si>
+    <t>&lt;b&gt;Переходим к разделу "Основания для разработки".&lt;/b&gt;\n\nВведите основания для разработки, это может быть, например, указ ректора или учебный план</t>
+  </si>
+  <si>
+    <t>&lt;b&gt;Переходим к разделу "Назначение разработки".&lt;/b&gt;\n\nВведите функциональное назначение</t>
+  </si>
+  <si>
+    <t>&lt;b&gt;Переходим к разделу "Требования к программе".&lt;/b&gt;\n\nВведите требования к составу выполняемых функций</t>
+  </si>
+  <si>
+    <t>&lt;b&gt;Переходим к разделу "Требования к документации".&lt;/b&gt;\n\nВведите специальные требования к программной документации</t>
+  </si>
+  <si>
+    <t>&lt;b&gt;Следующий раздел "Техникоэкономические показатели".&lt;/b&gt;\n\nОпишите ориентировочную экономическую эффективность</t>
+  </si>
+  <si>
+    <t>&lt;b&gt;Заполним сравнительную таблицу с аналогами.&lt;/b&gt;\n\nПо умолчанию она имеет вид таблицы с тремя аналогами и пятью сравнительными характеристиками. В итоговом файле вы сможете изменить их количество.\n\nВведите название первого аналога</t>
+  </si>
+  <si>
+    <t>&lt;b&gt;Седующий раздел "Порядок контроля и приемки".&lt;/b&gt;\n\nВведите виды испытаний</t>
+  </si>
+  <si>
+    <t>&lt;b&gt;Заключительный раздел "Список использованных источников".&lt;/b&gt;\n\nПо умолчанию в него включены 10 основных ГОСТ-ов, по которым оформляется техническое задание. Чтобы добавить свои источники, введите их через перевод строки в одном сообщении</t>
   </si>
 </sst>
 </file>
@@ -362,7 +362,7 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -684,8 +684,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90374932-3BD5-7B45-8650-D95A2EC64DDF}">
   <dimension ref="A1:D50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4:D50"/>
+    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
+      <selection activeCell="B52" sqref="B52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -721,7 +721,7 @@
         <v>43</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="C4" s="1" t="str">
         <f t="shared" ref="C4:C18" si="0">"'"&amp;A4&amp;"': '',"</f>
@@ -729,7 +729,7 @@
       </c>
       <c r="D4" s="1" t="str">
         <f t="shared" ref="D4:D18" si="1">"('"&amp;B4&amp;":', '"&amp;A4&amp;"'),"</f>
-        <v>('Сначала заполним титульный лист.\n\nВведите полное название ВУЗа, например "Национальный исследовательский университет Высшая Школа Экономики":', 'university'),</v>
+        <v>('&lt;b&gt;Сначала заполним титульный лист.&lt;/b&gt;\n\nВведите полное название ВУЗа, например "Национальный исследовательский университет Высшая Школа Экономики":', 'university'),</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -769,7 +769,7 @@
         <v>46</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>92</v>
+        <v>82</v>
       </c>
       <c r="C7" s="1" t="str">
         <f t="shared" si="0"/>
@@ -801,7 +801,7 @@
         <v>48</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="C9" s="1" t="str">
         <f t="shared" si="0"/>
@@ -849,7 +849,7 @@
         <v>51</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="C12" s="1" t="str">
         <f t="shared" si="0"/>
@@ -897,7 +897,7 @@
         <v>54</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>66</v>
+        <v>86</v>
       </c>
       <c r="C15" s="1" t="str">
         <f>"'"&amp;A15&amp;"': '',"</f>
@@ -905,7 +905,7 @@
       </c>
       <c r="D15" s="1" t="str">
         <f>"('"&amp;B15&amp;":', '"&amp;A15&amp;"'),"</f>
-        <v>('Переходим к заполнению раздела "Введение".\n\nНапишите краткую характеристику области применения программы, например "«Генератор документации ‘‘Радость Научника’’» — прикладная программа, разрабатываемая с целью облегчения формирования и оформления документации.":', 'brief_description'),</v>
+        <v>('&lt;b&gt;Переходим к заполнению раздела "Введение".&lt;/b&gt;\n\nНапишите краткую характеристику области применения программы, например "«Генератор документации ‘‘Радость Научника’’» — прикладная программа, разрабатываемая с целью облегчения формирования и оформления документации.":', 'brief_description'),</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="51" x14ac:dyDescent="0.2">
@@ -913,7 +913,7 @@
         <v>55</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>69</v>
+        <v>87</v>
       </c>
       <c r="C16" s="1" t="str">
         <f t="shared" si="0"/>
@@ -921,7 +921,7 @@
       </c>
       <c r="D16" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>('Переходим к разделу "Основания для разработки".\n\nВведите основания для разработки, это может быть, например, указ ректора или учебный план:', 'grounds_for_development'),</v>
+        <v>('&lt;b&gt;Переходим к разделу "Основания для разработки".&lt;/b&gt;\n\nВведите основания для разработки, это может быть, например, указ ректора или учебный план:', 'grounds_for_development'),</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -929,7 +929,7 @@
         <v>56</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>67</v>
+        <v>88</v>
       </c>
       <c r="C17" s="1" t="str">
         <f t="shared" si="0"/>
@@ -937,7 +937,7 @@
       </c>
       <c r="D17" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>('Переходим к разделу "Назначение разработки".\n\nВведите функциональное назначение:', 'functional_purpose'),</v>
+        <v>('&lt;b&gt;Переходим к разделу "Назначение разработки".&lt;/b&gt;\n\nВведите функциональное назначение:', 'functional_purpose'),</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -945,7 +945,7 @@
         <v>57</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C18" s="1" t="str">
         <f t="shared" si="0"/>
@@ -961,7 +961,7 @@
         <v>8</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>70</v>
+        <v>89</v>
       </c>
       <c r="C19" s="1" t="str">
         <f>"'"&amp;A19&amp;"': '',"</f>
@@ -969,15 +969,15 @@
       </c>
       <c r="D19" s="1" t="str">
         <f>"('"&amp;B19&amp;":', '"&amp;A19&amp;"'),"</f>
-        <v>('Переходим к разделу "Требования к программе".\n\nВведите требования к составу выполняемых функций:', 'requirements_functions_performed'),</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+        <v>('&lt;b&gt;Переходим к разделу "Требования к программе".&lt;/b&gt;\n\nВведите требования к составу выполняемых функций:', 'requirements_functions_performed'),</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="C20" s="1" t="str">
         <f t="shared" ref="C20:C50" si="2">"'"&amp;A20&amp;"': '',"</f>
@@ -988,12 +988,12 @@
         <v>('Введите требования к организации входных данных:', 'organization_input_data'),</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="C21" s="1" t="str">
         <f t="shared" si="2"/>
@@ -1036,12 +1036,12 @@
         <v>('Введите требования к интерфейсу:', 'interface_requirements'),</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
         <v>13</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C24" s="1" t="str">
         <f t="shared" si="2"/>
@@ -1052,12 +1052,12 @@
         <v>('Введите требования к контролю входной информации:', 'control_input_information'),</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
         <v>14</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="C25" s="1" t="str">
         <f t="shared" si="2"/>
@@ -1073,7 +1073,7 @@
         <v>15</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="C26" s="1" t="str">
         <f t="shared" si="2"/>
@@ -1084,12 +1084,12 @@
         <v>('Введите требования к восстановлению после отказа:', 'recovery_time'),</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="C27" s="1" t="str">
         <f t="shared" si="2"/>
@@ -1121,7 +1121,7 @@
         <v>18</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="C29" s="1" t="str">
         <f t="shared" si="2"/>
@@ -1249,7 +1249,7 @@
         <v>26</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>78</v>
+        <v>90</v>
       </c>
       <c r="C37" s="1" t="str">
         <f t="shared" si="2"/>
@@ -1257,15 +1257,15 @@
       </c>
       <c r="D37" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>('Переходим к разделу "Требования к документации".\n\nВведите специальные требования к программной документации:', 'special_requirements_for_documentation'),</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+        <v>('&lt;b&gt;Переходим к разделу "Требования к документации".&lt;/b&gt;\n\nВведите специальные требования к программной документации:', 'special_requirements_for_documentation'),</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
         <v>27</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>80</v>
+        <v>91</v>
       </c>
       <c r="C38" s="1" t="str">
         <f t="shared" si="2"/>
@@ -1273,7 +1273,7 @@
       </c>
       <c r="D38" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>('Следующий раздел "Техникоэкономические показатели"\n\nОпишите ориентировочную экономическую эффективность:', 'economic_efficiency'),</v>
+        <v>('&lt;b&gt;Следующий раздел "Техникоэкономические показатели".&lt;/b&gt;\n\nОпишите ориентировочную экономическую эффективность:', 'economic_efficiency'),</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -1281,7 +1281,7 @@
         <v>28</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="C39" s="1" t="str">
         <f t="shared" si="2"/>
@@ -1297,7 +1297,7 @@
         <v>0</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>81</v>
+        <v>92</v>
       </c>
       <c r="C40" s="1" t="str">
         <f t="shared" si="2"/>
@@ -1305,7 +1305,7 @@
       </c>
       <c r="D40" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>('Заполним сравнительную таблицу с аналогами. По умолчанию она имеет вид таблицы с тремя аналогами и пятью сравнительными характеристиками. В итоговом файле вы сможете изменить их количество.\n\nВведите название первого аналога:', 'analogue_1'),</v>
+        <v>('&lt;b&gt;Заполним сравнительную таблицу с аналогами.&lt;/b&gt;\n\nПо умолчанию она имеет вид таблицы с тремя аналогами и пятью сравнительными характеристиками. В итоговом файле вы сможете изменить их количество.\n\nВведите название первого аналога:', 'analogue_1'),</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -1313,7 +1313,7 @@
         <v>1</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="C41" s="1" t="str">
         <f t="shared" si="2"/>
@@ -1329,7 +1329,7 @@
         <v>2</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="C42" s="1" t="str">
         <f t="shared" si="2"/>
@@ -1345,7 +1345,7 @@
         <v>3</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="C43" s="1" t="str">
         <f t="shared" si="2"/>
@@ -1361,7 +1361,7 @@
         <v>4</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="C44" s="1" t="str">
         <f t="shared" si="2"/>
@@ -1377,7 +1377,7 @@
         <v>5</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="C45" s="1" t="str">
         <f t="shared" si="2"/>
@@ -1393,7 +1393,7 @@
         <v>6</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="C46" s="1" t="str">
         <f t="shared" si="2"/>
@@ -1409,7 +1409,7 @@
         <v>7</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="C47" s="1" t="str">
         <f t="shared" si="2"/>
@@ -1425,7 +1425,7 @@
         <v>29</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="C48" s="1" t="str">
         <f t="shared" si="2"/>
@@ -1433,7 +1433,7 @@
       </c>
       <c r="D48" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>('Седующий раздел "Порядок контроля и приемки".\n\nВведите виды испытаний:', 'types_of_tests'),</v>
+        <v>('&lt;b&gt;Седующий раздел "Порядок контроля и приемки".&lt;/b&gt;\n\nВведите виды испытаний:', 'types_of_tests'),</v>
       </c>
     </row>
     <row r="49" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -1452,12 +1452,12 @@
         <v>('Введите общие требования к приемке работы:', 'general_requirements_acceptance_of_work'),</v>
       </c>
     </row>
-    <row r="50" spans="1:4" ht="68" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:4" ht="85" x14ac:dyDescent="0.2">
       <c r="A50" s="2" t="s">
         <v>31</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="C50" s="1" t="str">
         <f t="shared" si="2"/>
@@ -1465,7 +1465,7 @@
       </c>
       <c r="D50" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>('Заключительный раздел "Список использованных источников".\n\nПо умолчанию в него включены 10 основных ГОСТ-ов, по которым оформляется техническое задание. Чтобы добавить свои источники, введите их через перевод строки в одном сообщении:', 'sources'),</v>
+        <v>('&lt;b&gt;Заключительный раздел "Список использованных источников".&lt;/b&gt;\n\nПо умолчанию в него включены 10 основных ГОСТ-ов, по которым оформляется техническое задание. Чтобы добавить свои источники, введите их через перевод строки в одном сообщении:', 'sources'),</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added the ability to convert to PDF
</commit_message>
<xml_diff>
--- a/словарьТЗ.xlsx
+++ b/словарьТЗ.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shapovv/PycharmProjects/Radost/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D2ACFAA-E34F-7A44-9FC0-90E6A99B09CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C299F9BA-F93E-AB43-9C3A-837A2D390F78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="18860" windowHeight="16840" xr2:uid="{5429B6A6-3AB4-3F43-B880-B81809A67136}"/>
   </bookViews>
@@ -684,8 +684,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90374932-3BD5-7B45-8650-D95A2EC64DDF}">
   <dimension ref="A1:D50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
-      <selection activeCell="B52" sqref="B52"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4:D50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
edited dictionary content for the title page
</commit_message>
<xml_diff>
--- a/словарьТЗ.xlsx
+++ b/словарьТЗ.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shapovv/PycharmProjects/Radost/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C299F9BA-F93E-AB43-9C3A-837A2D390F78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52650792-7256-0C42-BFB0-FDD4313427DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="18860" windowHeight="16840" xr2:uid="{5429B6A6-3AB4-3F43-B880-B81809A67136}"/>
+    <workbookView xWindow="12700" yWindow="500" windowWidth="16100" windowHeight="16840" activeTab="1" xr2:uid="{5429B6A6-3AB4-3F43-B880-B81809A67136}"/>
   </bookViews>
   <sheets>
-    <sheet name="Лист1" sheetId="1" r:id="rId1"/>
+    <sheet name="Техническое задание" sheetId="1" r:id="rId1"/>
+    <sheet name="Титульный лист" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="104">
   <si>
     <t>analogue_1</t>
   </si>
@@ -318,6 +319,34 @@
   </si>
   <si>
     <t>&lt;b&gt;Заключительный раздел "Список использованных источников".&lt;/b&gt;\n\nПо умолчанию в него включены 10 основных ГОСТ-ов, по которым оформляется техническое задание. Чтобы добавить свои источники, введите их через перевод строки в одном сообщении</t>
+  </si>
+  <si>
+    <t>project_type</t>
+  </si>
+  <si>
+    <t>Введите тип работы, например "Техническое задание"</t>
+  </si>
+  <si>
+    <t>supervisor_post</t>
+  </si>
+  <si>
+    <t>akad_post</t>
+  </si>
+  <si>
+    <t>Введите должность руководителя, согласовавшего документ, например "Научный руководитель, приглашенный преподаватель департамента программной инженерии"</t>
+  </si>
+  <si>
+    <t>Введите должность руководителя, утвердившего документ, например "Академический руководитель образовательной программы «Программная инженерия», кандидат
+технических наук"</t>
+  </si>
+  <si>
+    <t>Введите ФИО руководителя, утвердившего документ, в формате Фамилия И. О.</t>
+  </si>
+  <si>
+    <t>Введите ФИО руководителя, согласовавшего документ, в формате Фамилия И. О.</t>
+  </si>
+  <si>
+    <t>&lt;b&gt;Приступим к заполнению титульного листа.&lt;/b&gt;\n\nВведите полное название ВУЗа, например "Национальный исследовательский университет Высшая Школа Экономики"</t>
   </si>
 </sst>
 </file>
@@ -684,8 +713,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90374932-3BD5-7B45-8650-D95A2EC64DDF}">
   <dimension ref="A1:D50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4:D50"/>
+    <sheetView zoomScale="50" workbookViewId="0">
+      <selection sqref="A1:D51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -956,7 +985,7 @@
         <v>('Введите эксплуатационное назначение:', 'operational_purpose'),</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
         <v>8</v>
       </c>
@@ -1467,6 +1496,463 @@
         <f t="shared" si="3"/>
         <v>('&lt;b&gt;Заключительный раздел "Список использованных источников".&lt;/b&gt;\n\nПо умолчанию в него включены 10 основных ГОСТ-ов, по которым оформляется техническое задание. Чтобы добавить свои источники, введите их через перевод строки в одном сообщении:', 'sources'),</v>
       </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5EB27001-DFD3-CC4B-88F3-8FAF982AB5DB}">
+  <dimension ref="A1:D51"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="83" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4:D16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="29.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="60.33203125" customWidth="1"/>
+    <col min="3" max="3" width="16.83203125" customWidth="1"/>
+    <col min="4" max="4" width="79.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" s="1"/>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+    </row>
+    <row r="4" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="C4" s="1" t="str">
+        <f t="shared" ref="C4:C9" si="0">"'"&amp;A4&amp;"': '',"</f>
+        <v>'university': '',</v>
+      </c>
+      <c r="D4" s="1" t="str">
+        <f t="shared" ref="D4:D9" si="1">"('"&amp;B4&amp;":', '"&amp;A4&amp;"'),"</f>
+        <v>('&lt;b&gt;Приступим к заполнению титульного листа.&lt;/b&gt;\n\nВведите полное название ВУЗа, например "Национальный исследовательский университет Высшая Школа Экономики":', 'university'),</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C5" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>'faculty': '',</v>
+      </c>
+      <c r="D5" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>('Введите факультет, например "Факультет компьютерных наук":', 'faculty'),</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C6" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>'department': '',</v>
+      </c>
+      <c r="D6" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>('Введите департамент, например "Департамент программной инженерии":', 'department'),</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="C7" s="1" t="str">
+        <f t="shared" ref="C7" si="2">"'"&amp;A7&amp;"': '',"</f>
+        <v>'project_type': '',</v>
+      </c>
+      <c r="D7" s="1" t="str">
+        <f t="shared" ref="D7" si="3">"('"&amp;B7&amp;":', '"&amp;A7&amp;"'),"</f>
+        <v>('Введите тип работы, например "Техническое задание":', 'project_type'),</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="C8" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>'project_name': '',</v>
+      </c>
+      <c r="D8" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>('Введите название работы, например «Генератор документации "Радость Научника"»:', 'project_name'),</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="C9" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>'supervisor_post': '',</v>
+      </c>
+      <c r="D9" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>('Введите должность руководителя, согласовавшего документ, например "Научный руководитель, приглашенный преподаватель департамента программной инженерии":', 'supervisor_post'),</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="C10" s="1" t="str">
+        <f t="shared" ref="C10:C12" si="4">"'"&amp;A10&amp;"': '',"</f>
+        <v>'supervisor_name': '',</v>
+      </c>
+      <c r="D10" s="1" t="str">
+        <f t="shared" ref="D10:D12" si="5">"('"&amp;B10&amp;":', '"&amp;A10&amp;"'),"</f>
+        <v>('Введите ФИО руководителя, согласовавшего документ, в формате Фамилия И. О.:', 'supervisor_name'),</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="68" x14ac:dyDescent="0.2">
+      <c r="A11" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="C11" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>'akad_post': '',</v>
+      </c>
+      <c r="D11" s="1" t="str">
+        <f t="shared" si="5"/>
+        <v>('Введите должность руководителя, утвердившего документ, например "Академический руководитель образовательной программы «Программная инженерия», кандидат
+технических наук":', 'akad_post'),</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+      <c r="A12" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="C12" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>'akad_name': '',</v>
+      </c>
+      <c r="D12" s="1" t="str">
+        <f t="shared" si="5"/>
+        <v>('Введите ФИО руководителя, утвердившего документ, в формате Фамилия И. О.:', 'akad_name'),</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="102" x14ac:dyDescent="0.2">
+      <c r="A13" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="C13" s="1" t="str">
+        <f>"'"&amp;A13&amp;"': '',"</f>
+        <v>'number': '',</v>
+      </c>
+      <c r="D13" s="1" t="str">
+        <f>"('"&amp;B13&amp;":', '"&amp;A13&amp;"'),"</f>
+        <v>('Введите номер работы:\n\nПодсказка: в соотретствии с ГОСТ 19.103-77 "Обозначения программ и программных документов", номер имеет вид RU.12345678.123456-01, где RU - код страны, 12345678 - код организации-разработчик, 123456-01 - регистрационный номер, который присваивается в соответствии с ОКП.:', 'number'),</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A14" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C14" s="1" t="str">
+        <f>"'"&amp;A14&amp;"': '',"</f>
+        <v>'student_name': '',</v>
+      </c>
+      <c r="D14" s="1" t="str">
+        <f>"('"&amp;B14&amp;":', '"&amp;A14&amp;"'),"</f>
+        <v>('Введите ФИО исполнителя в формате Фамилия И. О.:', 'student_name'),</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A15" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C15" s="1" t="str">
+        <f>"'"&amp;A15&amp;"': '',"</f>
+        <v>'group_number': '',</v>
+      </c>
+      <c r="D15" s="1" t="str">
+        <f>"('"&amp;B15&amp;":', '"&amp;A15&amp;"'),"</f>
+        <v>('Введите номер группы, например "БПИ217":', 'group_number'),</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A16" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="C16" s="1" t="str">
+        <f>"'"&amp;A16&amp;"': '',"</f>
+        <v>'year': '',</v>
+      </c>
+      <c r="D16" s="1" t="str">
+        <f>"('"&amp;B16&amp;":', '"&amp;A16&amp;"'),"</f>
+        <v>('Введите год:', 'year'),</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" s="2"/>
+      <c r="B17" s="2"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" s="2"/>
+      <c r="B19" s="2"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" s="2"/>
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21" s="2"/>
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22" s="2"/>
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23" s="2"/>
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24" s="2"/>
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25" s="2"/>
+      <c r="B25" s="1"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26" s="2"/>
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A27" s="2"/>
+      <c r="B27" s="1"/>
+      <c r="C27" s="1"/>
+      <c r="D27" s="1"/>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A28" s="2"/>
+      <c r="B28" s="1"/>
+      <c r="C28" s="1"/>
+      <c r="D28" s="1"/>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A29" s="2"/>
+      <c r="B29" s="1"/>
+      <c r="C29" s="1"/>
+      <c r="D29" s="1"/>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A30" s="2"/>
+      <c r="B30" s="1"/>
+      <c r="C30" s="1"/>
+      <c r="D30" s="1"/>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A31" s="2"/>
+      <c r="B31" s="1"/>
+      <c r="C31" s="1"/>
+      <c r="D31" s="1"/>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A32" s="2"/>
+      <c r="B32" s="1"/>
+      <c r="C32" s="1"/>
+      <c r="D32" s="1"/>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A33" s="2"/>
+      <c r="B33" s="1"/>
+      <c r="C33" s="1"/>
+      <c r="D33" s="1"/>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A34" s="2"/>
+      <c r="B34" s="1"/>
+      <c r="C34" s="1"/>
+      <c r="D34" s="1"/>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A35" s="2"/>
+      <c r="B35" s="1"/>
+      <c r="C35" s="1"/>
+      <c r="D35" s="1"/>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A36" s="2"/>
+      <c r="B36" s="1"/>
+      <c r="C36" s="1"/>
+      <c r="D36" s="1"/>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A37" s="2"/>
+      <c r="B37" s="1"/>
+      <c r="C37" s="1"/>
+      <c r="D37" s="1"/>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A38" s="2"/>
+      <c r="B38" s="1"/>
+      <c r="C38" s="1"/>
+      <c r="D38" s="1"/>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A39" s="2"/>
+      <c r="B39" s="1"/>
+      <c r="C39" s="1"/>
+      <c r="D39" s="1"/>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A40" s="2"/>
+      <c r="B40" s="1"/>
+      <c r="C40" s="1"/>
+      <c r="D40" s="1"/>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A41" s="2"/>
+      <c r="B41" s="1"/>
+      <c r="C41" s="1"/>
+      <c r="D41" s="1"/>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A42" s="2"/>
+      <c r="B42" s="1"/>
+      <c r="C42" s="1"/>
+      <c r="D42" s="1"/>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A43" s="2"/>
+      <c r="B43" s="1"/>
+      <c r="C43" s="1"/>
+      <c r="D43" s="1"/>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A44" s="2"/>
+      <c r="B44" s="1"/>
+      <c r="C44" s="1"/>
+      <c r="D44" s="1"/>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A45" s="2"/>
+      <c r="B45" s="1"/>
+      <c r="C45" s="1"/>
+      <c r="D45" s="1"/>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A46" s="2"/>
+      <c r="B46" s="1"/>
+      <c r="C46" s="1"/>
+      <c r="D46" s="1"/>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A47" s="2"/>
+      <c r="B47" s="1"/>
+      <c r="C47" s="1"/>
+      <c r="D47" s="1"/>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A48" s="2"/>
+      <c r="B48" s="1"/>
+      <c r="C48" s="1"/>
+      <c r="D48" s="1"/>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A49" s="2"/>
+      <c r="B49" s="1"/>
+      <c r="C49" s="1"/>
+      <c r="D49" s="1"/>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A50" s="2"/>
+      <c r="B50" s="1"/>
+      <c r="C50" s="1"/>
+      <c r="D50" s="1"/>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A51" s="1"/>
+      <c r="B51" s="1"/>
+      <c r="C51" s="1"/>
+      <c r="D51" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
fixed errors in dictionaries
</commit_message>
<xml_diff>
--- a/словарьТЗ.xlsx
+++ b/словарьТЗ.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shapovv/PycharmProjects/Radost/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52650792-7256-0C42-BFB0-FDD4313427DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36B0E1D2-D04E-DD44-8CCE-49BF114E11C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12700" yWindow="500" windowWidth="16100" windowHeight="16840" activeTab="1" xr2:uid="{5429B6A6-3AB4-3F43-B880-B81809A67136}"/>
+    <workbookView xWindow="12700" yWindow="500" windowWidth="16100" windowHeight="16840" xr2:uid="{5429B6A6-3AB4-3F43-B880-B81809A67136}"/>
   </bookViews>
   <sheets>
     <sheet name="Техническое задание" sheetId="1" r:id="rId1"/>
@@ -231,9 +231,6 @@
     <t>Введите ФИО академического руководителя в формате Фамилия И. О.</t>
   </si>
   <si>
-    <t>Приступим к созданию вашего технического задания. Сейчас мы поэтапно пройдём по всем пунктам, начиная с титульного листа и заканчивая списком литературы. Следуйте дальнейшим указаниям и подсказкам. В любом месте вы можете остановиться и отправить ответ позднее, а если захотите закончить и получить документ с не до конца введёнными данными, введите /stop. Если вы хотите пропустить любой шаг, необходимо отправить в ответи любой символ, тогда вы сможете заполнить этот раздел самостоятельно в итоговом документе.</t>
-  </si>
-  <si>
     <t>Введите эксплуатационное назначение</t>
   </si>
   <si>
@@ -347,6 +344,9 @@
   </si>
   <si>
     <t>&lt;b&gt;Приступим к заполнению титульного листа.&lt;/b&gt;\n\nВведите полное название ВУЗа, например "Национальный исследовательский университет Высшая Школа Экономики"</t>
+  </si>
+  <si>
+    <t>&lt;b&gt;Приступим к созданию вашего технического задания.&lt;b&gt;\n Сейчас мы поэтапно пройдём по всем пунктам, начиная с титульного листа и заканчивая списком литературы. Следуйте дальнейшим указаниям и подсказкам. \n\nВ любом месте вы можете остановиться и отправить ответ позднее, а если захотите закончить и получить не док онца заполненный документ, введите /stop. \n\nЕсли вы хотите пропустить любой шаг, необходимо отправить в ответ любой символ, тогда вы сможете заполнить этот раздел самостоятельно в итоговом документе.</t>
   </si>
 </sst>
 </file>
@@ -713,8 +713,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90374932-3BD5-7B45-8650-D95A2EC64DDF}">
   <dimension ref="A1:D50"/>
   <sheetViews>
-    <sheetView zoomScale="50" workbookViewId="0">
-      <selection sqref="A1:D51"/>
+    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -740,7 +740,7 @@
     <row r="3" spans="1:4" ht="153" x14ac:dyDescent="0.2">
       <c r="A3" s="1"/>
       <c r="B3" s="1" t="s">
-        <v>65</v>
+        <v>103</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
@@ -750,7 +750,7 @@
         <v>43</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C4" s="1" t="str">
         <f t="shared" ref="C4:C18" si="0">"'"&amp;A4&amp;"': '',"</f>
@@ -798,7 +798,7 @@
         <v>46</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C7" s="1" t="str">
         <f t="shared" si="0"/>
@@ -830,7 +830,7 @@
         <v>48</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C9" s="1" t="str">
         <f t="shared" si="0"/>
@@ -878,7 +878,7 @@
         <v>51</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C12" s="1" t="str">
         <f t="shared" si="0"/>
@@ -926,7 +926,7 @@
         <v>54</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C15" s="1" t="str">
         <f>"'"&amp;A15&amp;"': '',"</f>
@@ -942,7 +942,7 @@
         <v>55</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C16" s="1" t="str">
         <f t="shared" si="0"/>
@@ -958,7 +958,7 @@
         <v>56</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C17" s="1" t="str">
         <f t="shared" si="0"/>
@@ -974,7 +974,7 @@
         <v>57</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C18" s="1" t="str">
         <f t="shared" si="0"/>
@@ -990,7 +990,7 @@
         <v>8</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C19" s="1" t="str">
         <f>"'"&amp;A19&amp;"': '',"</f>
@@ -1006,7 +1006,7 @@
         <v>9</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C20" s="1" t="str">
         <f t="shared" ref="C20:C50" si="2">"'"&amp;A20&amp;"': '',"</f>
@@ -1022,7 +1022,7 @@
         <v>10</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C21" s="1" t="str">
         <f t="shared" si="2"/>
@@ -1070,7 +1070,7 @@
         <v>13</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C24" s="1" t="str">
         <f t="shared" si="2"/>
@@ -1086,7 +1086,7 @@
         <v>14</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C25" s="1" t="str">
         <f t="shared" si="2"/>
@@ -1102,7 +1102,7 @@
         <v>15</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C26" s="1" t="str">
         <f t="shared" si="2"/>
@@ -1118,7 +1118,7 @@
         <v>16</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C27" s="1" t="str">
         <f t="shared" si="2"/>
@@ -1150,7 +1150,7 @@
         <v>18</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C29" s="1" t="str">
         <f t="shared" si="2"/>
@@ -1278,7 +1278,7 @@
         <v>26</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C37" s="1" t="str">
         <f t="shared" si="2"/>
@@ -1294,7 +1294,7 @@
         <v>27</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C38" s="1" t="str">
         <f t="shared" si="2"/>
@@ -1310,7 +1310,7 @@
         <v>28</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C39" s="1" t="str">
         <f t="shared" si="2"/>
@@ -1326,7 +1326,7 @@
         <v>0</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C40" s="1" t="str">
         <f t="shared" si="2"/>
@@ -1342,7 +1342,7 @@
         <v>1</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C41" s="1" t="str">
         <f t="shared" si="2"/>
@@ -1358,7 +1358,7 @@
         <v>2</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C42" s="1" t="str">
         <f t="shared" si="2"/>
@@ -1374,7 +1374,7 @@
         <v>3</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C43" s="1" t="str">
         <f t="shared" si="2"/>
@@ -1390,7 +1390,7 @@
         <v>4</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C44" s="1" t="str">
         <f t="shared" si="2"/>
@@ -1406,7 +1406,7 @@
         <v>5</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C45" s="1" t="str">
         <f t="shared" si="2"/>
@@ -1422,7 +1422,7 @@
         <v>6</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C46" s="1" t="str">
         <f t="shared" si="2"/>
@@ -1438,7 +1438,7 @@
         <v>7</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C47" s="1" t="str">
         <f t="shared" si="2"/>
@@ -1454,7 +1454,7 @@
         <v>29</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C48" s="1" t="str">
         <f t="shared" si="2"/>
@@ -1486,7 +1486,7 @@
         <v>31</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C50" s="1" t="str">
         <f t="shared" si="2"/>
@@ -1507,7 +1507,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5EB27001-DFD3-CC4B-88F3-8FAF982AB5DB}">
   <dimension ref="A1:D51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="83" workbookViewId="0">
+    <sheetView topLeftCell="B1" zoomScale="83" workbookViewId="0">
       <selection activeCell="D4" sqref="D4:D16"/>
     </sheetView>
   </sheetViews>
@@ -1542,7 +1542,7 @@
         <v>43</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C4" s="1" t="str">
         <f t="shared" ref="C4:C9" si="0">"'"&amp;A4&amp;"': '',"</f>
@@ -1585,12 +1585,12 @@
         <v>('Введите департамент, например "Департамент программной инженерии":', 'department'),</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>95</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>96</v>
       </c>
       <c r="C7" s="1" t="str">
         <f t="shared" ref="C7" si="2">"'"&amp;A7&amp;"': '',"</f>
@@ -1606,7 +1606,7 @@
         <v>46</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C8" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1619,10 +1619,10 @@
     </row>
     <row r="9" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C9" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1633,12 +1633,12 @@
         <v>('Введите должность руководителя, согласовавшего документ, например "Научный руководитель, приглашенный преподаватель департамента программной инженерии":', 'supervisor_post'),</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>52</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C10" s="1" t="str">
         <f t="shared" ref="C10:C12" si="4">"'"&amp;A10&amp;"': '',"</f>
@@ -1651,10 +1651,10 @@
     </row>
     <row r="11" spans="1:4" ht="68" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C11" s="1" t="str">
         <f t="shared" si="4"/>
@@ -1666,12 +1666,12 @@
 технических наук":', 'akad_post'),</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>53</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C12" s="1" t="str">
         <f t="shared" si="4"/>
@@ -1687,7 +1687,7 @@
         <v>48</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C13" s="1" t="str">
         <f>"'"&amp;A13&amp;"': '',"</f>
@@ -1735,7 +1735,7 @@
         <v>51</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C16" s="1" t="str">
         <f>"'"&amp;A16&amp;"': '',"</f>

</xml_diff>

<commit_message>
added illumination of the selected button
</commit_message>
<xml_diff>
--- a/словарьТЗ.xlsx
+++ b/словарьТЗ.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shapovv/PycharmProjects/Radost/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36B0E1D2-D04E-DD44-8CCE-49BF114E11C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5993A4E-553F-4048-B0E2-E3DBCD58E1D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="12700" yWindow="500" windowWidth="16100" windowHeight="16840" xr2:uid="{5429B6A6-3AB4-3F43-B880-B81809A67136}"/>
   </bookViews>
@@ -714,7 +714,7 @@
   <dimension ref="A1:D50"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
button lights and deactivation are configured
</commit_message>
<xml_diff>
--- a/словарьТЗ.xlsx
+++ b/словарьТЗ.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shapovv/PycharmProjects/Radost/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5993A4E-553F-4048-B0E2-E3DBCD58E1D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{821A6233-252D-AB40-A020-FD049BC97BF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12700" yWindow="500" windowWidth="16100" windowHeight="16840" xr2:uid="{5429B6A6-3AB4-3F43-B880-B81809A67136}"/>
+    <workbookView xWindow="1720" yWindow="500" windowWidth="27080" windowHeight="16840" activeTab="1" xr2:uid="{5429B6A6-3AB4-3F43-B880-B81809A67136}"/>
   </bookViews>
   <sheets>
     <sheet name="Техническое задание" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="105">
   <si>
     <t>analogue_1</t>
   </si>
@@ -343,10 +343,13 @@
     <t>Введите ФИО руководителя, согласовавшего документ, в формате Фамилия И. О.</t>
   </si>
   <si>
-    <t>&lt;b&gt;Приступим к заполнению титульного листа.&lt;/b&gt;\n\nВведите полное название ВУЗа, например "Национальный исследовательский университет Высшая Школа Экономики"</t>
-  </si>
-  <si>
     <t>&lt;b&gt;Приступим к созданию вашего технического задания.&lt;b&gt;\n Сейчас мы поэтапно пройдём по всем пунктам, начиная с титульного листа и заканчивая списком литературы. Следуйте дальнейшим указаниям и подсказкам. \n\nВ любом месте вы можете остановиться и отправить ответ позднее, а если захотите закончить и получить не док онца заполненный документ, введите /stop. \n\nЕсли вы хотите пропустить любой шаг, необходимо отправить в ответ любой символ, тогда вы сможете заполнить этот раздел самостоятельно в итоговом документе.</t>
+  </si>
+  <si>
+    <t>Введите полное название ВУЗа, например "Национальный исследовательский университет Высшая Школа Экономики"</t>
+  </si>
+  <si>
+    <t>&lt;b&gt;Приступим к созданию вашего титульного листа.&lt;b&gt;\n Сейчас мы поэтапно пройдём по всем пунктам, следуйте дальнейшим указаниям и подсказкам. \n\nВ любом месте вы можете остановиться и отправить ответ позднее, а если захотите закончить и получить не до конца заполненный документ, введите /stop. \n\nЕсли вы хотите пропустить любой шаг, необходимо отправить в ответ любой символ, тогда вы сможете заполнить этот раздел самостоятельно в итоговом документе.</t>
   </si>
 </sst>
 </file>
@@ -713,7 +716,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90374932-3BD5-7B45-8650-D95A2EC64DDF}">
   <dimension ref="A1:D50"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+    <sheetView zoomScale="150" workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -740,7 +743,7 @@
     <row r="3" spans="1:4" ht="153" x14ac:dyDescent="0.2">
       <c r="A3" s="1"/>
       <c r="B3" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
@@ -1507,8 +1510,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5EB27001-DFD3-CC4B-88F3-8FAF982AB5DB}">
   <dimension ref="A1:D51"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="83" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4:D16"/>
+    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1531,18 +1534,19 @@
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" ht="136" x14ac:dyDescent="0.2">
       <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
+      <c r="B3" s="1" t="s">
+        <v>104</v>
+      </c>
       <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
     </row>
     <row r="4" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>43</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C4" s="1" t="str">
         <f t="shared" ref="C4:C9" si="0">"'"&amp;A4&amp;"': '',"</f>
@@ -1550,7 +1554,7 @@
       </c>
       <c r="D4" s="1" t="str">
         <f t="shared" ref="D4:D9" si="1">"('"&amp;B4&amp;":', '"&amp;A4&amp;"'),"</f>
-        <v>('&lt;b&gt;Приступим к заполнению титульного листа.&lt;/b&gt;\n\nВведите полное название ВУЗа, например "Национальный исследовательский университет Высшая Школа Экономики":', 'university'),</v>
+        <v>('Введите полное название ВУЗа, например "Национальный исследовательский университет Высшая Школа Экономики":', 'university'),</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="17" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
updated dictionary for explanatory notes
</commit_message>
<xml_diff>
--- a/словарьТЗ.xlsx
+++ b/словарьТЗ.xlsx
@@ -8,15 +8,28 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shapovv/PycharmProjects/Radost/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6DE0CD5-736A-FC4F-A129-BDC7382A03A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC5A9533-6BB2-9941-AE90-536D0F275D5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="15480" windowHeight="16840" activeTab="2" xr2:uid="{5429B6A6-3AB4-3F43-B880-B81809A67136}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="24940" windowHeight="16840" activeTab="2" xr2:uid="{5429B6A6-3AB4-3F43-B880-B81809A67136}"/>
   </bookViews>
   <sheets>
     <sheet name="Техническое задание" sheetId="1" r:id="rId1"/>
     <sheet name="Титульный лист" sheetId="2" r:id="rId2"/>
     <sheet name="Пояснительная записка" sheetId="3" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="_Toc134566627" localSheetId="2">'Пояснительная записка'!$B$23</definedName>
+    <definedName name="_Toc134566629" localSheetId="2">'Пояснительная записка'!$B$24</definedName>
+    <definedName name="_Toc134566630" localSheetId="2">'Пояснительная записка'!$B$25</definedName>
+    <definedName name="_Toc134566632" localSheetId="2">'Пояснительная записка'!$B$26</definedName>
+    <definedName name="_Toc134566633" localSheetId="2">'Пояснительная записка'!$B$27</definedName>
+    <definedName name="_Toc134566634" localSheetId="2">'Пояснительная записка'!$B$28</definedName>
+    <definedName name="_Toc134566635" localSheetId="2">'Пояснительная записка'!$B$29</definedName>
+    <definedName name="_Toc134566637" localSheetId="2">'Пояснительная записка'!$B$30</definedName>
+    <definedName name="_Toc134566638" localSheetId="2">'Пояснительная записка'!$B$31</definedName>
+    <definedName name="_Toc134566640" localSheetId="2">'Пояснительная записка'!$B$32</definedName>
+    <definedName name="_Toc134566641" localSheetId="2">'Пояснительная записка'!$B$33</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -35,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="143">
   <si>
     <t>analogue_1</t>
   </si>
@@ -353,9 +366,6 @@
     <t>&lt;b&gt;Приступим к созданию вашего титульного листа.&lt;b&gt;\n Сейчас мы поэтапно пройдём по всем пунктам, следуйте дальнейшим указаниям и подсказкам. \n\nВ любом месте вы можете остановиться и отправить ответ позднее, а если захотите закончить и получить не до конца заполненный документ, введите /stop. \n\nЕсли вы хотите пропустить любой шаг, необходимо отправить в ответ любой символ, тогда вы сможете заполнить этот раздел самостоятельно в итоговом документе.</t>
   </si>
   <si>
-    <t>&lt;b&gt;Приступим к созданию вашей пояснительной записки.&lt;b&gt;\n Сейчас мы поэтапно пройдём по всем пунктам, начиная с титульного листа и заканчивая списком литературы. Следуйте дальнейшим указаниям и подсказкам. \n\nВ любом месте вы можете остановиться и отправить ответ позднее, а если захотите закончить и получить не док онца заполненный документ, введите /stop. \n\nЕсли вы хотите пропустить любой шаг, необходимо отправить в ответ любой символ, тогда вы сможете заполнить этот раздел самостоятельно в итоговом документе.</t>
-  </si>
-  <si>
     <t>&lt;b&gt;Переходим к заполнению раздела "Введение".&lt;/b&gt;\n\nВведите основания для разработки, это может быть, например, указ ректора или учебный план</t>
   </si>
   <si>
@@ -363,13 +373,118 @@
   </si>
   <si>
     <t>Напишите краткую характеристику области применения программы, например "«Генератор документации ‘‘Радость Научника’’» — прикладная программа, разрабатываемая с целью облегчения формирования и оформления документации."</t>
+  </si>
+  <si>
+    <t>month</t>
+  </si>
+  <si>
+    <t>day</t>
+  </si>
+  <si>
+    <t>Введите месяц в родительном падеже, например "Мая"</t>
+  </si>
+  <si>
+    <t>&lt;b&gt;Теперь заполнима дату, когда будет подписана пояснительная записка.&lt;/b&gt;\n\nВведите год, например "2023"</t>
+  </si>
+  <si>
+    <t>Введите число, например "11"</t>
+  </si>
+  <si>
+    <t>Введите номер работы:\n\nПодсказка: в соответствии с ГОСТ 19.103-77 "Обозначения программ и программных документов", номер имеет вид RU.12345678.123456-01, где RU - код страны, 12345678 - код организации-разработчик, 123456-01 - регистрационный номер, который присваивается в соответствии с ОКП.</t>
+  </si>
+  <si>
+    <t>Введите должность руководителя, утвердившего документ, например "Академический руководитель образовательной программы «Программная инженерия», кандидат технических наук"</t>
+  </si>
+  <si>
+    <t>task_statement</t>
+  </si>
+  <si>
+    <t>description_architecture</t>
+  </si>
+  <si>
+    <t>rationale_algorithm</t>
+  </si>
+  <si>
+    <t>composition_of_technical_means</t>
+  </si>
+  <si>
+    <t>advantages_over_analogues</t>
+  </si>
+  <si>
+    <t>term_1</t>
+  </si>
+  <si>
+    <t>definition_1</t>
+  </si>
+  <si>
+    <t>justification_of_architecture</t>
+  </si>
+  <si>
+    <t>description_algorithm</t>
+  </si>
+  <si>
+    <t>work_with_data_bases</t>
+  </si>
+  <si>
+    <t>input_output_data</t>
+  </si>
+  <si>
+    <t>justification_of_technical_means</t>
+  </si>
+  <si>
+    <t>perceived_need</t>
+  </si>
+  <si>
+    <t>&lt;b&gt;Переходим к разделу "Технические характеристики".&lt;/b&gt;\n\nОпишите поставленные задачи на разработку программы</t>
+  </si>
+  <si>
+    <t>Опишите архитектуру программы</t>
+  </si>
+  <si>
+    <t>Опишите алгоритм работы программы</t>
+  </si>
+  <si>
+    <t>Опишите работу с базами данных</t>
+  </si>
+  <si>
+    <t>Опишите и обоснуйте выбор способа организации входных и выходных данных</t>
+  </si>
+  <si>
+    <t>Опишите состав технических и программных средств</t>
+  </si>
+  <si>
+    <t>Обоснуйте выбор алгоритма работы программы</t>
+  </si>
+  <si>
+    <t>Обоснуйте выбор архитектуры программы</t>
+  </si>
+  <si>
+    <t>Обоснуйте выбор технических и программных средств</t>
+  </si>
+  <si>
+    <t>Опишите экономические преимущества разработки по сравнению с отечественными и зарубежными аналогами</t>
+  </si>
+  <si>
+    <t>&lt;b&gt;Переходим к разделу "Список использованных источников".&lt;/b&gt;\n\nПо умолчанию в него включены 12 основных ГОСТ-ов, по которым оформляется пояснительная записка. Чтобы добавить свои источники, введите их через перевод строки в одном сообщении</t>
+  </si>
+  <si>
+    <t>&lt;b&gt;Наконец заполним одно из приложений в качестве примера.&lt;/b&gt;\n\nНе забудьте дозаполнить таблицы, которые генерируются по умолчанию в приложениях. Вы сможете после сохранения документа в формате .docx.\n\nВведите любой технический термин из текста вашей пояснительной записки</t>
+  </si>
+  <si>
+    <t>Введите определение введенного выше термина</t>
+  </si>
+  <si>
+    <t>&lt;b&gt;Переходим к разделу "Ожидаемые технико-экономические показатели".&lt;/b&gt;\n\nОпишите ориентировочную экономическую эффективность</t>
+  </si>
+  <si>
+    <t>&lt;b&gt;Приступим к созданию вашей пояснительной записки.&lt;/b&gt;\nСейчас мы поэтапно пройдём по всем пунктам, начиная с титульного листа и заканчивая списком литературы. Следуйте дальнейшим указаниям и подсказкам. \n\nВ любом месте вы можете остановиться и отправить ответ позднее, а если захотите закончить и получить не до конца заполненный документ, введите /stop. \n\nЕсли вы хотите пропустить любой шаг, необходимо отправить в ответ любой символ, тогда вы сможете заполнить этот раздел самостоятельно в итоговом документе.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -381,6 +496,17 @@
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
@@ -405,13 +531,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -729,8 +861,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90374932-3BD5-7B45-8650-D95A2EC64DDF}">
   <dimension ref="A1:D50"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="90" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15:B15"/>
+    <sheetView topLeftCell="A34" zoomScale="90" workbookViewId="0">
+      <selection activeCell="B50" sqref="B50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1523,8 +1655,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5EB27001-DFD3-CC4B-88F3-8FAF982AB5DB}">
   <dimension ref="A1:D51"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="125" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView topLeftCell="A12" zoomScale="125" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11:XFD11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1979,10 +2111,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFD8DD06-B0A9-7C4D-BF4B-D4D05FDA4F57}">
-  <dimension ref="A1:D52"/>
+  <dimension ref="A1:D56"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4:D18"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2008,7 +2140,7 @@
     <row r="3" spans="1:4" ht="187" x14ac:dyDescent="0.2">
       <c r="A3" s="1"/>
       <c r="B3" s="1" t="s">
-        <v>105</v>
+        <v>142</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
@@ -2021,11 +2153,11 @@
         <v>84</v>
       </c>
       <c r="C4" s="1" t="str">
-        <f t="shared" ref="C4:C17" si="0">"'"&amp;A4&amp;"': '',"</f>
+        <f t="shared" ref="C4:C15" si="0">"'"&amp;A4&amp;"': '',"</f>
         <v>'university': '',</v>
       </c>
       <c r="D4" s="1" t="str">
-        <f t="shared" ref="D4:D17" si="1">"('"&amp;B4&amp;":', '"&amp;A4&amp;"'),"</f>
+        <f t="shared" ref="D4:D15" si="1">"('"&amp;B4&amp;":', '"&amp;A4&amp;"'),"</f>
         <v>('&lt;b&gt;Сначала заполним титульный лист.&lt;/b&gt;\n\nВведите полное название ВУЗа, например "Национальный исследовательский университет Высшая Школа Экономики":', 'university'),</v>
       </c>
     </row>
@@ -2098,7 +2230,7 @@
         <v>48</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>82</v>
+        <v>113</v>
       </c>
       <c r="C9" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2106,676 +2238,570 @@
       </c>
       <c r="D9" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>('Введите номер работы:\n\nПодсказка: в соотретствии с ГОСТ 19.103-77 "Обозначения программ и программных документов", номер имеет вид RU.12345678.123456-01, где RU - код страны, 12345678 - код организации-разработчик, 123456-01 - регистрационный номер, который присваивается в соответствии с ОКП.:', 'number'),</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+        <v>('Введите номер работы:\n\nПодсказка: в соответствии с ГОСТ 19.103-77 "Обозначения программ и программных документов", номер имеет вид RU.12345678.123456-01, где RU - код страны, 12345678 - код организации-разработчик, 123456-01 - регистрационный номер, который присваивается в соответствии с ОКП.:', 'number'),</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="68" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="C10" s="1" t="str">
+        <f t="shared" ref="C10" si="2">"'"&amp;A10&amp;"': '',"</f>
+        <v>'supervisor_post': '',</v>
+      </c>
+      <c r="D10" s="1" t="str">
+        <f t="shared" ref="D10" si="3">"('"&amp;B10&amp;":', '"&amp;A10&amp;"'),"</f>
+        <v>('Введите должность руководителя, согласовавшего документ, например "Научный руководитель, приглашенный преподаватель департамента программной инженерии":', 'supervisor_post'),</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A11" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C11" s="1" t="str">
+        <f>"'"&amp;A11&amp;"': '',"</f>
+        <v>'supervisor_name': '',</v>
+      </c>
+      <c r="D11" s="1" t="str">
+        <f>"('"&amp;B11&amp;":', '"&amp;A11&amp;"'),"</f>
+        <v>('Введите ФИО научного руководителя в формате Фамилия И. О.:', 'supervisor_name'),</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="68" x14ac:dyDescent="0.2">
+      <c r="A12" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="C12" s="1" t="str">
+        <f t="shared" ref="C12" si="4">"'"&amp;A12&amp;"': '',"</f>
+        <v>'akad_post': '',</v>
+      </c>
+      <c r="D12" s="1" t="str">
+        <f t="shared" ref="D12" si="5">"('"&amp;B12&amp;":', '"&amp;A12&amp;"'),"</f>
+        <v>('Введите должность руководителя, утвердившего документ, например "Академический руководитель образовательной программы «Программная инженерия», кандидат технических наук":', 'akad_post'),</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A13" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C13" s="1" t="str">
+        <f>"'"&amp;A13&amp;"': '',"</f>
+        <v>'akad_name': '',</v>
+      </c>
+      <c r="D13" s="1" t="str">
+        <f>"('"&amp;B13&amp;":', '"&amp;A13&amp;"'),"</f>
+        <v>('Введите ФИО академического руководителя в формате Фамилия И. О.:', 'akad_name'),</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A14" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B14" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="C10" s="1" t="str">
+      <c r="C14" s="1" t="str">
         <f t="shared" si="0"/>
         <v>'student_name': '',</v>
       </c>
-      <c r="D10" s="1" t="str">
+      <c r="D14" s="1" t="str">
         <f t="shared" si="1"/>
         <v>('Введите ФИО исполнителя в формате Фамилия И. О.:', 'student_name'),</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A11" s="2" t="s">
+    <row r="15" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A15" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B15" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="C11" s="1" t="str">
+      <c r="C15" s="1" t="str">
         <f t="shared" si="0"/>
         <v>'group_number': '',</v>
       </c>
-      <c r="D11" s="1" t="str">
+      <c r="D15" s="1" t="str">
         <f t="shared" si="1"/>
         <v>('Введите номер группы, например "БПИ217":', 'group_number'),</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A12" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="C12" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>'year': '',</v>
-      </c>
-      <c r="D12" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>('Введите год:', 'year'),</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A13" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="C13" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>'supervisor_name': '',</v>
-      </c>
-      <c r="D13" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>('Введите ФИО научного руководителя в формате Фамилия И. О.:', 'supervisor_name'),</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A14" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="C14" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>'akad_name': '',</v>
-      </c>
-      <c r="D14" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>('Введите ФИО академического руководителя в формате Фамилия И. О.:', 'akad_name'),</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="68" x14ac:dyDescent="0.2">
-      <c r="A15" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="C15" s="1" t="str">
-        <f>"'"&amp;A15&amp;"': '',"</f>
-        <v>'grounds_for_development': '',</v>
-      </c>
-      <c r="D15" s="1" t="str">
-        <f>"('"&amp;B15&amp;":', '"&amp;A15&amp;"'),"</f>
-        <v>('&lt;b&gt;Переходим к заполнению раздела "Введение".&lt;/b&gt;\n\nВведите основания для разработки, это может быть, например, указ ректора или учебный план:', 'grounds_for_development'),</v>
-      </c>
-    </row>
     <row r="16" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="C16" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>'functional_purpose': '',</v>
+        <f>"'"&amp;A16&amp;"': '',"</f>
+        <v>'year': '',</v>
       </c>
       <c r="D16" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>('&lt;b&gt;Переходим к разделу "Назначение и область применения".&lt;/b&gt;\n\nВведите функциональное назначение:', 'functional_purpose'),</v>
+        <f>"('"&amp;B16&amp;":', '"&amp;A16&amp;"'),"</f>
+        <v>('&lt;b&gt;Теперь заполнима дату, когда будет подписана пояснительная записка.&lt;/b&gt;\n\nВведите год, например "2023":', 'year'),</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="C17" s="1" t="str">
+        <f>"'"&amp;A17&amp;"': '',"</f>
+        <v>'month': '',</v>
+      </c>
+      <c r="D17" s="1" t="str">
+        <f>"('"&amp;B17&amp;":', '"&amp;A17&amp;"'),"</f>
+        <v>('Введите месяц в родительном падеже, например "Мая":', 'month'),</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A18" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="C18" s="1" t="str">
+        <f>"'"&amp;A18&amp;"': '',"</f>
+        <v>'day': '',</v>
+      </c>
+      <c r="D18" s="1" t="str">
+        <f>"('"&amp;B18&amp;":', '"&amp;A18&amp;"'),"</f>
+        <v>('Введите число, например "11":', 'day'),</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="68" x14ac:dyDescent="0.2">
+      <c r="A19" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="C19" s="1" t="str">
+        <f>"'"&amp;A19&amp;"': '',"</f>
+        <v>'grounds_for_development': '',</v>
+      </c>
+      <c r="D19" s="1" t="str">
+        <f>"('"&amp;B19&amp;":', '"&amp;A19&amp;"'),"</f>
+        <v>('&lt;b&gt;Переходим к заполнению раздела "Введение".&lt;/b&gt;\n\nВведите основания для разработки, это может быть, например, указ ректора или учебный план:', 'grounds_for_development'),</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+      <c r="A20" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="C20" s="1" t="str">
+        <f>"'"&amp;A20&amp;"': '',"</f>
+        <v>'functional_purpose': '',</v>
+      </c>
+      <c r="D20" s="1" t="str">
+        <f>"('"&amp;B20&amp;":', '"&amp;A20&amp;"'),"</f>
+        <v>('&lt;b&gt;Переходим к разделу "Назначение и область применения".&lt;/b&gt;\n\nВведите функциональное назначение:', 'functional_purpose'),</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A21" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="B21" s="2" t="s">
         <v>65</v>
-      </c>
-      <c r="C17" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>'operational_purpose': '',</v>
-      </c>
-      <c r="D17" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>('Введите эксплуатационное назначение:', 'operational_purpose'),</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="85" x14ac:dyDescent="0.2">
-      <c r="A18" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="C18" s="1" t="str">
-        <f t="shared" ref="C18" si="2">"'"&amp;A18&amp;"': '',"</f>
-        <v>'brief_description': '',</v>
-      </c>
-      <c r="D18" s="1" t="str">
-        <f t="shared" ref="D18" si="3">"('"&amp;B18&amp;":', '"&amp;A18&amp;"'),"</f>
-        <v>('Напишите краткую характеристику области применения программы, например "«Генератор документации ‘‘Радость Научника’’» — прикладная программа, разрабатываемая с целью облегчения формирования и оформления документации.":', 'brief_description'),</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="113" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="2"/>
-      <c r="B19" s="2"/>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A20" s="2"/>
-      <c r="B20" s="2"/>
-      <c r="C20" s="1"/>
-      <c r="D20" s="1"/>
-    </row>
-    <row r="21" spans="1:4" ht="51" x14ac:dyDescent="0.2">
-      <c r="A21" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>88</v>
       </c>
       <c r="C21" s="1" t="str">
         <f>"'"&amp;A21&amp;"': '',"</f>
-        <v>'requirements_functions_performed': '',</v>
+        <v>'operational_purpose': '',</v>
       </c>
       <c r="D21" s="1" t="str">
         <f>"('"&amp;B21&amp;":', '"&amp;A21&amp;"'),"</f>
-        <v>('&lt;b&gt;Переходим к разделу "Требования к программе".&lt;/b&gt;\n\nВведите требования к составу выполняемых функций:', 'requirements_functions_performed'),</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+        <v>('Введите эксплуатационное назначение:', 'operational_purpose'),</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="85" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>66</v>
+        <v>54</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>107</v>
       </c>
       <c r="C22" s="1" t="str">
-        <f t="shared" ref="C22:C52" si="4">"'"&amp;A22&amp;"': '',"</f>
-        <v>'organization_input_data': '',</v>
+        <f>"'"&amp;A22&amp;"': '',"</f>
+        <v>'brief_description': '',</v>
       </c>
       <c r="D22" s="1" t="str">
-        <f t="shared" ref="D22:D52" si="5">"('"&amp;B22&amp;":', '"&amp;A22&amp;"'),"</f>
-        <v>('Введите требования к организации входных данных:', 'organization_input_data'),</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A23" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>67</v>
+        <f>"('"&amp;B22&amp;":', '"&amp;A22&amp;"'),"</f>
+        <v>('Напишите краткую характеристику области применения программы, например "«Генератор документации ‘‘Радость Научника’’» — прикладная программа, разрабатываемая с целью облегчения формирования и оформления документации.":', 'brief_description'),</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="68" x14ac:dyDescent="0.2">
+      <c r="A23" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>128</v>
       </c>
       <c r="C23" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>'organization_output_data': '',</v>
+        <f t="shared" ref="C23:C38" si="6">"'"&amp;A23&amp;"': '',"</f>
+        <v>'task_statement': '',</v>
       </c>
       <c r="D23" s="1" t="str">
-        <f t="shared" si="5"/>
-        <v>('Введите требования организация выходных данных:', 'organization_output_data'),</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A24" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>32</v>
+        <f t="shared" ref="D23:D38" si="7">"('"&amp;B23&amp;":', '"&amp;A23&amp;"'),"</f>
+        <v>('&lt;b&gt;Переходим к разделу "Технические характеристики".&lt;/b&gt;\n\nОпишите поставленные задачи на разработку программы:', 'task_statement'),</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="68" x14ac:dyDescent="0.2">
+      <c r="A24" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>129</v>
       </c>
       <c r="C24" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>'requirements_time': '',</v>
+        <f t="shared" si="6"/>
+        <v>'description_architecture': '',</v>
       </c>
       <c r="D24" s="1" t="str">
-        <f t="shared" si="5"/>
-        <v>('Введите требования к временным характеристикам:', 'requirements_time'),</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A25" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>33</v>
+        <f t="shared" si="7"/>
+        <v>('Опишите архитектуру программы:', 'description_architecture'),</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="68" x14ac:dyDescent="0.2">
+      <c r="A25" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>135</v>
       </c>
       <c r="C25" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>'interface_requirements': '',</v>
+        <f t="shared" si="6"/>
+        <v>'justification_of_architecture': '',</v>
       </c>
       <c r="D25" s="1" t="str">
-        <f t="shared" si="5"/>
-        <v>('Введите требования к интерфейсу:', 'interface_requirements'),</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A26" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>68</v>
+        <f t="shared" si="7"/>
+        <v>('Обоснуйте выбор архитектуры программы:', 'justification_of_architecture'),</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="68" x14ac:dyDescent="0.2">
+      <c r="A26" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>130</v>
       </c>
       <c r="C26" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>'control_input_information': '',</v>
+        <f t="shared" si="6"/>
+        <v>'description_algorithm': '',</v>
       </c>
       <c r="D26" s="1" t="str">
-        <f t="shared" si="5"/>
-        <v>('Введите требования к контролю входной информации:', 'control_input_information'),</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A27" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>69</v>
+        <f t="shared" si="7"/>
+        <v>('Опишите алгоритм работы программы:', 'description_algorithm'),</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="68" x14ac:dyDescent="0.2">
+      <c r="A27" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>134</v>
       </c>
       <c r="C27" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>'control_output_information': '',</v>
+        <f t="shared" si="6"/>
+        <v>'rationale_algorithm': '',</v>
       </c>
       <c r="D27" s="1" t="str">
-        <f t="shared" si="5"/>
-        <v>('Введите требования к контролю выходной информации:', 'control_output_information'),</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A28" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>70</v>
+        <f t="shared" si="7"/>
+        <v>('Обоснуйте выбор алгоритма работы программы:', 'rationale_algorithm'),</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="68" x14ac:dyDescent="0.2">
+      <c r="A28" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>131</v>
       </c>
       <c r="C28" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>'recovery_time': '',</v>
+        <f t="shared" si="6"/>
+        <v>'work_with_data_bases': '',</v>
       </c>
       <c r="D28" s="1" t="str">
-        <f t="shared" si="5"/>
-        <v>('Введите требования к восстановлению после отказа:', 'recovery_time'),</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A29" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>71</v>
+        <f t="shared" si="7"/>
+        <v>('Опишите работу с базами данных:', 'work_with_data_bases'),</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="68" x14ac:dyDescent="0.2">
+      <c r="A29" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>132</v>
       </c>
       <c r="C29" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>'climatic_conditions': '',</v>
+        <f t="shared" si="6"/>
+        <v>'input_output_data': '',</v>
       </c>
       <c r="D29" s="1" t="str">
-        <f t="shared" si="5"/>
-        <v>('Введите требования к климатическим условиям эксплуатации:', 'climatic_conditions'),</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A30" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>34</v>
+        <f t="shared" si="7"/>
+        <v>('Опишите и обоснуйте выбор способа организации входных и выходных данных:', 'input_output_data'),</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="68" x14ac:dyDescent="0.2">
+      <c r="A30" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>133</v>
       </c>
       <c r="C30" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>'types_services': '',</v>
+        <f t="shared" si="6"/>
+        <v>'composition_of_technical_means': '',</v>
       </c>
       <c r="D30" s="1" t="str">
-        <f t="shared" si="5"/>
-        <v>('Введите требования к видам обсулживания:', 'types_services'),</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A31" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>72</v>
+        <f t="shared" si="7"/>
+        <v>('Опишите состав технических и программных средств:', 'composition_of_technical_means'),</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="68" x14ac:dyDescent="0.2">
+      <c r="A31" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>136</v>
       </c>
       <c r="C31" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>'number_and_qual_personnel': '',</v>
+        <f t="shared" si="6"/>
+        <v>'justification_of_technical_means': '',</v>
       </c>
       <c r="D31" s="1" t="str">
-        <f t="shared" si="5"/>
-        <v>('Введите требования к численности и квалификации персонала:', 'number_and_qual_personnel'),</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A32" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>35</v>
+        <f t="shared" si="7"/>
+        <v>('Обоснуйте выбор технических и программных средств:', 'justification_of_technical_means'),</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+      <c r="A32" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>141</v>
       </c>
       <c r="C32" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>'parameters_technical_means': '',</v>
+        <f t="shared" si="6"/>
+        <v>'economic_efficiency': '',</v>
       </c>
       <c r="D32" s="1" t="str">
-        <f t="shared" si="5"/>
-        <v>('Введите требования к составу и параметрам технических средств:', 'parameters_technical_means'),</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A33" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>36</v>
+        <f t="shared" si="7"/>
+        <v>('&lt;b&gt;Переходим к разделу "Ожидаемые технико-экономические показатели".&lt;/b&gt;\n\nОпишите ориентировочную экономическую эффективность:', 'economic_efficiency'),</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="68" x14ac:dyDescent="0.2">
+      <c r="A33" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>73</v>
       </c>
       <c r="C33" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>'programming_languages': '',</v>
+        <f t="shared" si="6"/>
+        <v>'perceived_need': '',</v>
       </c>
       <c r="D33" s="1" t="str">
-        <f t="shared" si="5"/>
-        <v>('Введите требования к исходным кодам и языкам программирования:', 'programming_languages'),</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A34" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>37</v>
+        <f t="shared" si="7"/>
+        <v>('Опишите предполагаемую потребность:', 'perceived_need'),</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="68" x14ac:dyDescent="0.2">
+      <c r="A34" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B34" s="4" t="s">
+        <v>137</v>
       </c>
       <c r="C34" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>'software': '',</v>
+        <f t="shared" si="6"/>
+        <v>'advantages_over_analogues': '',</v>
       </c>
       <c r="D34" s="1" t="str">
-        <f t="shared" si="5"/>
-        <v>('Введите требования к программным средствам, используемым программой:', 'software'),</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A35" s="2" t="s">
-        <v>22</v>
+        <f t="shared" si="7"/>
+        <v>('Опишите экономические преимущества разработки по сравнению с отечественными и зарубежными аналогами:', 'advantages_over_analogues'),</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="102" x14ac:dyDescent="0.2">
+      <c r="A35" s="1" t="s">
+        <v>31</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>38</v>
+        <v>138</v>
       </c>
       <c r="C35" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>'protection_information': '',</v>
+        <f t="shared" si="6"/>
+        <v>'sources': '',</v>
       </c>
       <c r="D35" s="1" t="str">
-        <f t="shared" si="5"/>
-        <v>('Введите требования к защите информации и программ:', 'protection_information'),</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A36" s="2" t="s">
-        <v>23</v>
+        <f t="shared" si="7"/>
+        <v>('&lt;b&gt;Переходим к разделу "Список использованных источников".&lt;/b&gt;\n\nПо умолчанию в него включены 12 основных ГОСТ-ов, по которым оформляется пояснительная записка. Чтобы добавить свои источники, введите их через перевод строки в одном сообщении:', 'sources'),</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="119" x14ac:dyDescent="0.2">
+      <c r="A36" s="1" t="s">
+        <v>120</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>39</v>
+        <v>139</v>
       </c>
       <c r="C36" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>'labeling_and_packaging': '',</v>
+        <f t="shared" si="6"/>
+        <v>'term_1': '',</v>
       </c>
       <c r="D36" s="1" t="str">
-        <f t="shared" si="5"/>
-        <v>('Введите требования к маркировке и упаковке:', 'labeling_and_packaging'),</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A37" s="2" t="s">
-        <v>24</v>
+        <f t="shared" si="7"/>
+        <v>('&lt;b&gt;Наконец заполним одно из приложений в качестве примера.&lt;/b&gt;\n\nНе забудьте дозаполнить таблицы, которые генерируются по умолчанию в приложениях. Вы сможете после сохранения документа в формате .docx.\n\nВведите любой технический термин из текста вашей пояснительной записки:', 'term_1'),</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" ht="68" x14ac:dyDescent="0.2">
+      <c r="A37" s="1" t="s">
+        <v>121</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>40</v>
+        <v>140</v>
       </c>
       <c r="C37" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>'transportation_and_storage': '',</v>
+        <f t="shared" si="6"/>
+        <v>'definition_1': '',</v>
       </c>
       <c r="D37" s="1" t="str">
-        <f t="shared" si="5"/>
-        <v>('Введите требования к транспортированию и хранению:', 'transportation_and_storage'),</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A38" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B38" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C38" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>'special_requirements': '',</v>
-      </c>
-      <c r="D38" s="1" t="str">
-        <f t="shared" si="5"/>
-        <v>('Введите специальные требования:', 'special_requirements'),</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" ht="51" x14ac:dyDescent="0.2">
-      <c r="A39" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B39" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="C39" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>'special_requirements_for_documentation': '',</v>
-      </c>
-      <c r="D39" s="1" t="str">
-        <f t="shared" si="5"/>
-        <v>('&lt;b&gt;Переходим к разделу "Требования к документации".&lt;/b&gt;\n\nВведите специальные требования к программной документации:', 'special_requirements_for_documentation'),</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" ht="51" x14ac:dyDescent="0.2">
-      <c r="A40" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B40" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="C40" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>'economic_efficiency': '',</v>
-      </c>
-      <c r="D40" s="1" t="str">
-        <f t="shared" si="5"/>
-        <v>('&lt;b&gt;Следующий раздел "Техникоэкономические показатели".&lt;/b&gt;\n\nОпишите ориентировочную экономическую эффективность:', 'economic_efficiency'),</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A41" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B41" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="C41" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>'estimated_need': '',</v>
-      </c>
-      <c r="D41" s="1" t="str">
-        <f t="shared" si="5"/>
-        <v>('Опишите предполагаемую потребность:', 'estimated_need'),</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" ht="102" x14ac:dyDescent="0.2">
-      <c r="A42" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B42" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="C42" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>'analogue_1': '',</v>
-      </c>
-      <c r="D42" s="1" t="str">
-        <f t="shared" si="5"/>
-        <v>('&lt;b&gt;Заполним сравнительную таблицу с аналогами.&lt;/b&gt;\n\nПо умолчанию она имеет вид таблицы с тремя аналогами и пятью сравнительными характеристиками. В итоговом файле вы сможете изменить их количество.\n\nВведите название первого аналога:', 'analogue_1'),</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A43" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B43" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="C43" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>'analogue_2': '',</v>
-      </c>
-      <c r="D43" s="1" t="str">
-        <f t="shared" si="5"/>
-        <v>('Введите название второго аналога:', 'analogue_2'),</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A44" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B44" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="C44" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>'analogue_3': '',</v>
-      </c>
-      <c r="D44" s="1" t="str">
-        <f t="shared" si="5"/>
-        <v>('Введите название третьего аналога:', 'analogue_3'),</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A45" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B45" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="C45" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>'characteristic_1': '',</v>
-      </c>
-      <c r="D45" s="1" t="str">
-        <f t="shared" si="5"/>
-        <v>('Введите первую сравнительную характеристику:', 'characteristic_1'),</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A46" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B46" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="C46" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>'characteristic_2': '',</v>
-      </c>
-      <c r="D46" s="1" t="str">
-        <f t="shared" si="5"/>
-        <v>('Введите вторую сравнительную характеристику:', 'characteristic_2'),</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A47" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B47" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="C47" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>'characteristic_3': '',</v>
-      </c>
-      <c r="D47" s="1" t="str">
-        <f t="shared" si="5"/>
-        <v>('Введите третью сравнительную характеристику:', 'characteristic_3'),</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A48" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B48" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="C48" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>'characteristic_4': '',</v>
-      </c>
-      <c r="D48" s="1" t="str">
-        <f t="shared" si="5"/>
-        <v>('Введите четвертую сравнительную характеристику:', 'characteristic_4'),</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A49" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B49" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="C49" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>'characteristic_5': '',</v>
-      </c>
-      <c r="D49" s="1" t="str">
-        <f t="shared" si="5"/>
-        <v>('Введите пятую сравнительную характеристику:', 'characteristic_5'),</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A50" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="B50" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="C50" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>'types_of_tests': '',</v>
-      </c>
-      <c r="D50" s="1" t="str">
-        <f t="shared" si="5"/>
-        <v>('&lt;b&gt;Седующий раздел "Порядок контроля и приемки".&lt;/b&gt;\n\nВведите виды испытаний:', 'types_of_tests'),</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A51" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B51" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="C51" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>'general_requirements_acceptance_of_work': '',</v>
-      </c>
-      <c r="D51" s="1" t="str">
-        <f t="shared" si="5"/>
-        <v>('Введите общие требования к приемке работы:', 'general_requirements_acceptance_of_work'),</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" ht="102" x14ac:dyDescent="0.2">
-      <c r="A52" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B52" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="C52" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>'sources': '',</v>
-      </c>
-      <c r="D52" s="1" t="str">
-        <f t="shared" si="5"/>
-        <v>('&lt;b&gt;Заключительный раздел "Список использованных источников".&lt;/b&gt;\n\nПо умолчанию в него включены 10 основных ГОСТ-ов, по которым оформляется техническое задание. Чтобы добавить свои источники, введите их через перевод строки в одном сообщении:', 'sources'),</v>
-      </c>
+        <f t="shared" si="7"/>
+        <v>('Введите определение введенного выше термина:', 'definition_1'),</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A38" s="2"/>
+      <c r="B38" s="1"/>
+      <c r="C38" s="1"/>
+      <c r="D38" s="1"/>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A39" s="2"/>
+      <c r="B39" s="1"/>
+      <c r="C39" s="1"/>
+      <c r="D39" s="1"/>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A40" s="2"/>
+      <c r="B40" s="1"/>
+      <c r="C40" s="1"/>
+      <c r="D40" s="1"/>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A41" s="2"/>
+      <c r="B41" s="1"/>
+      <c r="C41" s="1"/>
+      <c r="D41" s="1"/>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A42" s="2"/>
+      <c r="B42" s="1"/>
+      <c r="C42" s="1"/>
+      <c r="D42" s="1"/>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A43" s="2"/>
+      <c r="B43" s="1"/>
+      <c r="C43" s="1"/>
+      <c r="D43" s="1"/>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A44" s="2"/>
+      <c r="B44" s="1"/>
+      <c r="C44" s="1"/>
+      <c r="D44" s="1"/>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A45" s="2"/>
+      <c r="B45" s="1"/>
+      <c r="C45" s="1"/>
+      <c r="D45" s="1"/>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A46" s="2"/>
+      <c r="B46" s="1"/>
+      <c r="C46" s="1"/>
+      <c r="D46" s="1"/>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A47" s="2"/>
+      <c r="B47" s="1"/>
+      <c r="C47" s="1"/>
+      <c r="D47" s="1"/>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A48" s="2"/>
+      <c r="B48" s="1"/>
+      <c r="C48" s="1"/>
+      <c r="D48" s="1"/>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A49" s="2"/>
+      <c r="B49" s="1"/>
+      <c r="C49" s="1"/>
+      <c r="D49" s="1"/>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A50" s="2"/>
+      <c r="B50" s="1"/>
+      <c r="C50" s="1"/>
+      <c r="D50" s="1"/>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A51" s="2"/>
+      <c r="B51" s="1"/>
+      <c r="C51" s="1"/>
+      <c r="D51" s="1"/>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A52" s="2"/>
+      <c r="B52" s="1"/>
+      <c r="C52" s="1"/>
+      <c r="D52" s="1"/>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A53" s="2"/>
+      <c r="B53" s="1"/>
+      <c r="C53" s="1"/>
+      <c r="D53" s="1"/>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A54" s="2"/>
+      <c r="B54" s="1"/>
+      <c r="C54" s="1"/>
+      <c r="D54" s="1"/>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A55" s="2"/>
+      <c r="B55" s="1"/>
+      <c r="C55" s="1"/>
+      <c r="D55" s="1"/>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A56" s="2"/>
+      <c r="B56" s="1"/>
+      <c r="C56" s="1"/>
+      <c r="D56" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
parallel operation and correct file names are configured
</commit_message>
<xml_diff>
--- a/словарьТЗ.xlsx
+++ b/словарьТЗ.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shapovv/PycharmProjects/Radost/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC5A9533-6BB2-9941-AE90-536D0F275D5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16827391-E752-E547-B542-00852CF996EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="24940" windowHeight="16840" activeTab="2" xr2:uid="{5429B6A6-3AB4-3F43-B880-B81809A67136}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="24940" windowHeight="16840" activeTab="1" xr2:uid="{5429B6A6-3AB4-3F43-B880-B81809A67136}"/>
   </bookViews>
   <sheets>
     <sheet name="Техническое задание" sheetId="1" r:id="rId1"/>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="144">
   <si>
     <t>analogue_1</t>
   </si>
@@ -347,10 +347,6 @@
     <t>Введите должность руководителя, согласовавшего документ, например "Научный руководитель, приглашенный преподаватель департамента программной инженерии"</t>
   </si>
   <si>
-    <t>Введите должность руководителя, утвердившего документ, например "Академический руководитель образовательной программы «Программная инженерия», кандидат
-технических наук"</t>
-  </si>
-  <si>
     <t>Введите ФИО руководителя, утвердившего документ, в формате Фамилия И. О.</t>
   </si>
   <si>
@@ -478,6 +474,12 @@
   </si>
   <si>
     <t>&lt;b&gt;Приступим к созданию вашей пояснительной записки.&lt;/b&gt;\nСейчас мы поэтапно пройдём по всем пунктам, начиная с титульного листа и заканчивая списком литературы. Следуйте дальнейшим указаниям и подсказкам. \n\nВ любом месте вы можете остановиться и отправить ответ позднее, а если захотите закончить и получить не до конца заполненный документ, введите /stop. \n\nЕсли вы хотите пропустить любой шаг, необходимо отправить в ответ любой символ, тогда вы сможете заполнить этот раздел самостоятельно в итоговом документе.</t>
+  </si>
+  <si>
+    <t>second_name</t>
+  </si>
+  <si>
+    <t>Введите Фамилию на английском языке, например "Shapovalov"</t>
   </si>
 </sst>
 </file>
@@ -888,7 +890,7 @@
     <row r="3" spans="1:4" ht="153" x14ac:dyDescent="0.2">
       <c r="A3" s="1"/>
       <c r="B3" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
@@ -1653,10 +1655,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5EB27001-DFD3-CC4B-88F3-8FAF982AB5DB}">
-  <dimension ref="A1:D51"/>
+  <dimension ref="A1:D53"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" zoomScale="125" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11:XFD11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1682,244 +1684,241 @@
     <row r="3" spans="1:4" ht="136" x14ac:dyDescent="0.2">
       <c r="A3" s="1"/>
       <c r="B3" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C3" s="1"/>
     </row>
-    <row r="4" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>103</v>
+        <v>83</v>
       </c>
       <c r="C4" s="1" t="str">
-        <f t="shared" ref="C4:C9" si="0">"'"&amp;A4&amp;"': '',"</f>
-        <v>'university': '',</v>
+        <f>"'"&amp;A4&amp;"': '',"</f>
+        <v>'year': '',</v>
       </c>
       <c r="D4" s="1" t="str">
-        <f t="shared" ref="D4:D9" si="1">"('"&amp;B4&amp;":', '"&amp;A4&amp;"'),"</f>
-        <v>('Введите полное название ВУЗа, например "Национальный исследовательский университет Высшая Школа Экономики":', 'university'),</v>
+        <f>"('"&amp;B4&amp;":', '"&amp;A4&amp;"'),"</f>
+        <v>('Введите год:', 'year'),</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="C5" s="1" t="str">
+        <f>"'"&amp;A5&amp;"': '',"</f>
+        <v>'second_name': '',</v>
+      </c>
+      <c r="D5" s="1" t="str">
+        <f>"('"&amp;B5&amp;":', '"&amp;A5&amp;"'),"</f>
+        <v>('Введите Фамилию на английском языке, например "Shapovalov":', 'second_name'),</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="C6" s="1" t="str">
+        <f t="shared" ref="C6:C11" si="0">"'"&amp;A6&amp;"': '',"</f>
+        <v>'university': '',</v>
+      </c>
+      <c r="D6" s="1" t="str">
+        <f t="shared" ref="D6:D11" si="1">"('"&amp;B6&amp;":', '"&amp;A6&amp;"'),"</f>
+        <v>('Введите полное название ВУЗа, например "Национальный исследовательский университет Высшая Школа Экономики":', 'university'),</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B7" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="C5" s="1" t="str">
+      <c r="C7" s="1" t="str">
         <f t="shared" si="0"/>
         <v>'faculty': '',</v>
       </c>
-      <c r="D5" s="1" t="str">
+      <c r="D7" s="1" t="str">
         <f t="shared" si="1"/>
         <v>('Введите факультет, например "Факультет компьютерных наук":', 'faculty'),</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A6" s="2" t="s">
+    <row r="8" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B8" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="C6" s="1" t="str">
+      <c r="C8" s="1" t="str">
         <f t="shared" si="0"/>
         <v>'department': '',</v>
       </c>
-      <c r="D6" s="1" t="str">
+      <c r="D8" s="1" t="str">
         <f t="shared" si="1"/>
         <v>('Введите департамент, например "Департамент программной инженерии":', 'department'),</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A7" s="2" t="s">
+    <row r="9" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B9" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="C7" s="1" t="str">
-        <f t="shared" ref="C7" si="2">"'"&amp;A7&amp;"': '',"</f>
+      <c r="C9" s="1" t="str">
+        <f t="shared" ref="C9" si="2">"'"&amp;A9&amp;"': '',"</f>
         <v>'project_type': '',</v>
       </c>
-      <c r="D7" s="1" t="str">
-        <f t="shared" ref="D7" si="3">"('"&amp;B7&amp;":', '"&amp;A7&amp;"'),"</f>
+      <c r="D9" s="1" t="str">
+        <f t="shared" ref="D9" si="3">"('"&amp;B9&amp;":', '"&amp;A9&amp;"'),"</f>
         <v>('Введите тип работы, например "Техническое задание":', 'project_type'),</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A8" s="2" t="s">
+    <row r="10" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B10" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="C8" s="1" t="str">
+      <c r="C10" s="1" t="str">
         <f t="shared" si="0"/>
         <v>'project_name': '',</v>
       </c>
-      <c r="D8" s="1" t="str">
+      <c r="D10" s="1" t="str">
         <f t="shared" si="1"/>
         <v>('Введите название работы, например «Генератор документации "Радость Научника"»:', 'project_name'),</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="51" x14ac:dyDescent="0.2">
-      <c r="A9" s="2" t="s">
+    <row r="11" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+      <c r="A11" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B11" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="C9" s="1" t="str">
+      <c r="C11" s="1" t="str">
         <f t="shared" si="0"/>
         <v>'supervisor_post': '',</v>
       </c>
-      <c r="D9" s="1" t="str">
+      <c r="D11" s="1" t="str">
         <f t="shared" si="1"/>
         <v>('Введите должность руководителя, согласовавшего документ, например "Научный руководитель, приглашенный преподаватель департамента программной инженерии":', 'supervisor_post'),</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A10" s="2" t="s">
+    <row r="12" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A12" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B10" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="C10" s="1" t="str">
-        <f t="shared" ref="C10:C12" si="4">"'"&amp;A10&amp;"': '',"</f>
+      <c r="B12" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="C12" s="1" t="str">
+        <f t="shared" ref="C12:C14" si="4">"'"&amp;A12&amp;"': '',"</f>
         <v>'supervisor_name': '',</v>
       </c>
-      <c r="D10" s="1" t="str">
-        <f t="shared" ref="D10:D12" si="5">"('"&amp;B10&amp;":', '"&amp;A10&amp;"'),"</f>
+      <c r="D12" s="1" t="str">
+        <f t="shared" ref="D12:D14" si="5">"('"&amp;B12&amp;":', '"&amp;A12&amp;"'),"</f>
         <v>('Введите ФИО руководителя, согласовавшего документ, в формате Фамилия И. О.:', 'supervisor_name'),</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="68" x14ac:dyDescent="0.2">
-      <c r="A11" s="2" t="s">
+    <row r="13" spans="1:4" ht="68" x14ac:dyDescent="0.2">
+      <c r="A13" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="B11" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="C11" s="1" t="str">
+      <c r="B13" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="C13" s="1" t="str">
         <f t="shared" si="4"/>
         <v>'akad_post': '',</v>
       </c>
-      <c r="D11" s="1" t="str">
+      <c r="D13" s="1" t="str">
         <f t="shared" si="5"/>
-        <v>('Введите должность руководителя, утвердившего документ, например "Академический руководитель образовательной программы «Программная инженерия», кандидат
-технических наук":', 'akad_post'),</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A12" s="2" t="s">
+        <v>('Введите должность руководителя, утвердившего документ, например "Академический руководитель образовательной программы «Программная инженерия», кандидат технических наук":', 'akad_post'),</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A14" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="B12" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="C12" s="1" t="str">
+      <c r="B14" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="C14" s="1" t="str">
         <f t="shared" si="4"/>
         <v>'akad_name': '',</v>
       </c>
-      <c r="D12" s="1" t="str">
+      <c r="D14" s="1" t="str">
         <f t="shared" si="5"/>
         <v>('Введите ФИО руководителя, утвердившего документ, в формате Фамилия И. О.:', 'akad_name'),</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="102" x14ac:dyDescent="0.2">
-      <c r="A13" s="2" t="s">
+    <row r="15" spans="1:4" ht="102" x14ac:dyDescent="0.2">
+      <c r="A15" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B15" s="2" t="s">
         <v>82</v>
-      </c>
-      <c r="C13" s="1" t="str">
-        <f>"'"&amp;A13&amp;"': '',"</f>
-        <v>'number': '',</v>
-      </c>
-      <c r="D13" s="1" t="str">
-        <f>"('"&amp;B13&amp;":', '"&amp;A13&amp;"'),"</f>
-        <v>('Введите номер работы:\n\nПодсказка: в соотретствии с ГОСТ 19.103-77 "Обозначения программ и программных документов", номер имеет вид RU.12345678.123456-01, где RU - код страны, 12345678 - код организации-разработчик, 123456-01 - регистрационный номер, который присваивается в соответствии с ОКП.:', 'number'),</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A14" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="C14" s="1" t="str">
-        <f>"'"&amp;A14&amp;"': '',"</f>
-        <v>'student_name': '',</v>
-      </c>
-      <c r="D14" s="1" t="str">
-        <f>"('"&amp;B14&amp;":', '"&amp;A14&amp;"'),"</f>
-        <v>('Введите ФИО исполнителя в формате Фамилия И. О.:', 'student_name'),</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A15" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>62</v>
       </c>
       <c r="C15" s="1" t="str">
         <f>"'"&amp;A15&amp;"': '',"</f>
-        <v>'group_number': '',</v>
+        <v>'number': '',</v>
       </c>
       <c r="D15" s="1" t="str">
         <f>"('"&amp;B15&amp;":', '"&amp;A15&amp;"'),"</f>
-        <v>('Введите номер группы, например "БПИ217":', 'group_number'),</v>
+        <v>('Введите номер работы:\n\nПодсказка: в соотретствии с ГОСТ 19.103-77 "Обозначения программ и программных документов", номер имеет вид RU.12345678.123456-01, где RU - код страны, 12345678 - код организации-разработчик, 123456-01 - регистрационный номер, который присваивается в соответствии с ОКП.:', 'number'),</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>83</v>
+        <v>61</v>
       </c>
       <c r="C16" s="1" t="str">
         <f>"'"&amp;A16&amp;"': '',"</f>
-        <v>'year': '',</v>
+        <v>'student_name': '',</v>
       </c>
       <c r="D16" s="1" t="str">
         <f>"('"&amp;B16&amp;":', '"&amp;A16&amp;"'),"</f>
-        <v>('Введите год:', 'year'),</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17" s="2"/>
-      <c r="B17" s="2"/>
-      <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="C18" s="1"/>
-      <c r="D18" s="1"/>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A19" s="2"/>
-      <c r="B19" s="2"/>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
+        <v>('Введите ФИО исполнителя в формате Фамилия И. О.:', 'student_name'),</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A17" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C17" s="1" t="str">
+        <f>"'"&amp;A17&amp;"': '',"</f>
+        <v>'group_number': '',</v>
+      </c>
+      <c r="D17" s="1" t="str">
+        <f>"('"&amp;B17&amp;":', '"&amp;A17&amp;"'),"</f>
+        <v>('Введите номер группы, например "БПИ217":', 'group_number'),</v>
+      </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A20" s="2"/>
-      <c r="B20" s="1"/>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" s="2"/>
-      <c r="B21" s="1"/>
+      <c r="B21" s="2"/>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
     </row>
@@ -2098,10 +2097,22 @@
       <c r="D50" s="1"/>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A51" s="1"/>
+      <c r="A51" s="2"/>
       <c r="B51" s="1"/>
       <c r="C51" s="1"/>
       <c r="D51" s="1"/>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A52" s="2"/>
+      <c r="B52" s="1"/>
+      <c r="C52" s="1"/>
+      <c r="D52" s="1"/>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A53" s="1"/>
+      <c r="B53" s="1"/>
+      <c r="C53" s="1"/>
+      <c r="D53" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2113,7 +2124,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFD8DD06-B0A9-7C4D-BF4B-D4D05FDA4F57}">
   <dimension ref="A1:D56"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A24" workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -2140,7 +2151,7 @@
     <row r="3" spans="1:4" ht="187" x14ac:dyDescent="0.2">
       <c r="A3" s="1"/>
       <c r="B3" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
@@ -2230,7 +2241,7 @@
         <v>48</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C9" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2278,7 +2289,7 @@
         <v>97</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C12" s="1" t="str">
         <f t="shared" ref="C12" si="4">"'"&amp;A12&amp;"': '',"</f>
@@ -2342,46 +2353,46 @@
         <v>51</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C16" s="1" t="str">
-        <f>"'"&amp;A16&amp;"': '',"</f>
+        <f t="shared" ref="C16:C22" si="6">"'"&amp;A16&amp;"': '',"</f>
         <v>'year': '',</v>
       </c>
       <c r="D16" s="1" t="str">
-        <f>"('"&amp;B16&amp;":', '"&amp;A16&amp;"'),"</f>
+        <f t="shared" ref="D16:D22" si="7">"('"&amp;B16&amp;":', '"&amp;A16&amp;"'),"</f>
         <v>('&lt;b&gt;Теперь заполнима дату, когда будет подписана пояснительная записка.&lt;/b&gt;\n\nВведите год, например "2023":', 'year'),</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C17" s="1" t="str">
-        <f>"'"&amp;A17&amp;"': '',"</f>
+        <f t="shared" si="6"/>
         <v>'month': '',</v>
       </c>
       <c r="D17" s="1" t="str">
-        <f>"('"&amp;B17&amp;":', '"&amp;A17&amp;"'),"</f>
+        <f t="shared" si="7"/>
         <v>('Введите месяц в родительном падеже, например "Мая":', 'month'),</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C18" s="1" t="str">
-        <f>"'"&amp;A18&amp;"': '',"</f>
+        <f t="shared" si="6"/>
         <v>'day': '',</v>
       </c>
       <c r="D18" s="1" t="str">
-        <f>"('"&amp;B18&amp;":', '"&amp;A18&amp;"'),"</f>
+        <f t="shared" si="7"/>
         <v>('Введите число, например "11":', 'day'),</v>
       </c>
     </row>
@@ -2390,14 +2401,14 @@
         <v>55</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C19" s="1" t="str">
-        <f>"'"&amp;A19&amp;"': '',"</f>
+        <f t="shared" si="6"/>
         <v>'grounds_for_development': '',</v>
       </c>
       <c r="D19" s="1" t="str">
-        <f>"('"&amp;B19&amp;":', '"&amp;A19&amp;"'),"</f>
+        <f t="shared" si="7"/>
         <v>('&lt;b&gt;Переходим к заполнению раздела "Введение".&lt;/b&gt;\n\nВведите основания для разработки, это может быть, например, указ ректора или учебный план:', 'grounds_for_development'),</v>
       </c>
     </row>
@@ -2406,14 +2417,14 @@
         <v>56</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C20" s="1" t="str">
-        <f>"'"&amp;A20&amp;"': '',"</f>
+        <f t="shared" si="6"/>
         <v>'functional_purpose': '',</v>
       </c>
       <c r="D20" s="1" t="str">
-        <f>"('"&amp;B20&amp;":', '"&amp;A20&amp;"'),"</f>
+        <f t="shared" si="7"/>
         <v>('&lt;b&gt;Переходим к разделу "Назначение и область применения".&lt;/b&gt;\n\nВведите функциональное назначение:', 'functional_purpose'),</v>
       </c>
     </row>
@@ -2425,11 +2436,11 @@
         <v>65</v>
       </c>
       <c r="C21" s="1" t="str">
-        <f>"'"&amp;A21&amp;"': '',"</f>
+        <f t="shared" si="6"/>
         <v>'operational_purpose': '',</v>
       </c>
       <c r="D21" s="1" t="str">
-        <f>"('"&amp;B21&amp;":', '"&amp;A21&amp;"'),"</f>
+        <f t="shared" si="7"/>
         <v>('Введите эксплуатационное назначение:', 'operational_purpose'),</v>
       </c>
     </row>
@@ -2438,158 +2449,158 @@
         <v>54</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C22" s="1" t="str">
-        <f>"'"&amp;A22&amp;"': '',"</f>
+        <f t="shared" si="6"/>
         <v>'brief_description': '',</v>
       </c>
       <c r="D22" s="1" t="str">
-        <f>"('"&amp;B22&amp;":', '"&amp;A22&amp;"'),"</f>
+        <f t="shared" si="7"/>
         <v>('Напишите краткую характеристику области применения программы, например "«Генератор документации ‘‘Радость Научника’’» — прикладная программа, разрабатываемая с целью облегчения формирования и оформления документации.":', 'brief_description'),</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="68" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="C23" s="1" t="str">
+        <f t="shared" ref="C23:C37" si="8">"'"&amp;A23&amp;"': '',"</f>
+        <v>'task_statement': '',</v>
+      </c>
+      <c r="D23" s="1" t="str">
+        <f t="shared" ref="D23:D37" si="9">"('"&amp;B23&amp;":', '"&amp;A23&amp;"'),"</f>
+        <v>('&lt;b&gt;Переходим к разделу "Технические характеристики".&lt;/b&gt;\n\nОпишите поставленные задачи на разработку программы:', 'task_statement'),</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A24" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="B23" s="3" t="s">
+      <c r="B24" s="4" t="s">
         <v>128</v>
       </c>
-      <c r="C23" s="1" t="str">
-        <f t="shared" ref="C23:C38" si="6">"'"&amp;A23&amp;"': '',"</f>
-        <v>'task_statement': '',</v>
-      </c>
-      <c r="D23" s="1" t="str">
-        <f t="shared" ref="D23:D38" si="7">"('"&amp;B23&amp;":', '"&amp;A23&amp;"'),"</f>
-        <v>('&lt;b&gt;Переходим к разделу "Технические характеристики".&lt;/b&gt;\n\nОпишите поставленные задачи на разработку программы:', 'task_statement'),</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" ht="68" x14ac:dyDescent="0.2">
-      <c r="A24" s="1" t="s">
+      <c r="C24" s="1" t="str">
+        <f t="shared" si="8"/>
+        <v>'description_architecture': '',</v>
+      </c>
+      <c r="D24" s="1" t="str">
+        <f t="shared" si="9"/>
+        <v>('Опишите архитектуру программы:', 'description_architecture'),</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A25" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="C25" s="1" t="str">
+        <f t="shared" si="8"/>
+        <v>'justification_of_architecture': '',</v>
+      </c>
+      <c r="D25" s="1" t="str">
+        <f t="shared" si="9"/>
+        <v>('Обоснуйте выбор архитектуры программы:', 'justification_of_architecture'),</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A26" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="C26" s="1" t="str">
+        <f t="shared" si="8"/>
+        <v>'description_algorithm': '',</v>
+      </c>
+      <c r="D26" s="1" t="str">
+        <f t="shared" si="9"/>
+        <v>('Опишите алгоритм работы программы:', 'description_algorithm'),</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A27" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="B24" s="4" t="s">
-        <v>129</v>
-      </c>
-      <c r="C24" s="1" t="str">
-        <f t="shared" si="6"/>
-        <v>'description_architecture': '',</v>
-      </c>
-      <c r="D24" s="1" t="str">
-        <f t="shared" si="7"/>
-        <v>('Опишите архитектуру программы:', 'description_architecture'),</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" ht="68" x14ac:dyDescent="0.2">
-      <c r="A25" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="B25" s="4" t="s">
+      <c r="B27" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="C27" s="1" t="str">
+        <f t="shared" si="8"/>
+        <v>'rationale_algorithm': '',</v>
+      </c>
+      <c r="D27" s="1" t="str">
+        <f t="shared" si="9"/>
+        <v>('Обоснуйте выбор алгоритма работы программы:', 'rationale_algorithm'),</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A28" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="C28" s="1" t="str">
+        <f t="shared" si="8"/>
+        <v>'work_with_data_bases': '',</v>
+      </c>
+      <c r="D28" s="1" t="str">
+        <f t="shared" si="9"/>
+        <v>('Опишите работу с базами данных:', 'work_with_data_bases'),</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A29" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="C29" s="1" t="str">
+        <f t="shared" si="8"/>
+        <v>'input_output_data': '',</v>
+      </c>
+      <c r="D29" s="1" t="str">
+        <f t="shared" si="9"/>
+        <v>('Опишите и обоснуйте выбор способа организации входных и выходных данных:', 'input_output_data'),</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A30" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="C30" s="1" t="str">
+        <f t="shared" si="8"/>
+        <v>'composition_of_technical_means': '',</v>
+      </c>
+      <c r="D30" s="1" t="str">
+        <f t="shared" si="9"/>
+        <v>('Опишите состав технических и программных средств:', 'composition_of_technical_means'),</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A31" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="B31" s="4" t="s">
         <v>135</v>
       </c>
-      <c r="C25" s="1" t="str">
-        <f t="shared" si="6"/>
-        <v>'justification_of_architecture': '',</v>
-      </c>
-      <c r="D25" s="1" t="str">
-        <f t="shared" si="7"/>
-        <v>('Обоснуйте выбор архитектуры программы:', 'justification_of_architecture'),</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" ht="68" x14ac:dyDescent="0.2">
-      <c r="A26" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="B26" s="4" t="s">
-        <v>130</v>
-      </c>
-      <c r="C26" s="1" t="str">
-        <f t="shared" si="6"/>
-        <v>'description_algorithm': '',</v>
-      </c>
-      <c r="D26" s="1" t="str">
-        <f t="shared" si="7"/>
-        <v>('Опишите алгоритм работы программы:', 'description_algorithm'),</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" ht="68" x14ac:dyDescent="0.2">
-      <c r="A27" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="B27" s="4" t="s">
-        <v>134</v>
-      </c>
-      <c r="C27" s="1" t="str">
-        <f t="shared" si="6"/>
-        <v>'rationale_algorithm': '',</v>
-      </c>
-      <c r="D27" s="1" t="str">
-        <f t="shared" si="7"/>
-        <v>('Обоснуйте выбор алгоритма работы программы:', 'rationale_algorithm'),</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" ht="68" x14ac:dyDescent="0.2">
-      <c r="A28" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="B28" s="4" t="s">
-        <v>131</v>
-      </c>
-      <c r="C28" s="1" t="str">
-        <f t="shared" si="6"/>
-        <v>'work_with_data_bases': '',</v>
-      </c>
-      <c r="D28" s="1" t="str">
-        <f t="shared" si="7"/>
-        <v>('Опишите работу с базами данных:', 'work_with_data_bases'),</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" ht="68" x14ac:dyDescent="0.2">
-      <c r="A29" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="B29" s="4" t="s">
-        <v>132</v>
-      </c>
-      <c r="C29" s="1" t="str">
-        <f t="shared" si="6"/>
-        <v>'input_output_data': '',</v>
-      </c>
-      <c r="D29" s="1" t="str">
-        <f t="shared" si="7"/>
-        <v>('Опишите и обоснуйте выбор способа организации входных и выходных данных:', 'input_output_data'),</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" ht="68" x14ac:dyDescent="0.2">
-      <c r="A30" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="B30" s="4" t="s">
-        <v>133</v>
-      </c>
-      <c r="C30" s="1" t="str">
-        <f t="shared" si="6"/>
-        <v>'composition_of_technical_means': '',</v>
-      </c>
-      <c r="D30" s="1" t="str">
-        <f t="shared" si="7"/>
-        <v>('Опишите состав технических и программных средств:', 'composition_of_technical_means'),</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" ht="68" x14ac:dyDescent="0.2">
-      <c r="A31" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="B31" s="4" t="s">
-        <v>136</v>
-      </c>
       <c r="C31" s="1" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>'justification_of_technical_means': '',</v>
       </c>
       <c r="D31" s="1" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>('Обоснуйте выбор технических и программных средств:', 'justification_of_technical_means'),</v>
       </c>
     </row>
@@ -2598,46 +2609,46 @@
         <v>27</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C32" s="1" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>'economic_efficiency': '',</v>
       </c>
       <c r="D32" s="1" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>('&lt;b&gt;Переходим к разделу "Ожидаемые технико-экономические показатели".&lt;/b&gt;\n\nОпишите ориентировочную экономическую эффективность:', 'economic_efficiency'),</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="68" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B33" s="4" t="s">
         <v>73</v>
       </c>
       <c r="C33" s="1" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>'perceived_need': '',</v>
       </c>
       <c r="D33" s="1" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>('Опишите предполагаемую потребность:', 'perceived_need'),</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="68" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C34" s="1" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>'advantages_over_analogues': '',</v>
       </c>
       <c r="D34" s="1" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>('Опишите экономические преимущества разработки по сравнению с отечественными и зарубежными аналогами:', 'advantages_over_analogues'),</v>
       </c>
     </row>
@@ -2646,46 +2657,46 @@
         <v>31</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C35" s="1" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>'sources': '',</v>
       </c>
       <c r="D35" s="1" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>('&lt;b&gt;Переходим к разделу "Список использованных источников".&lt;/b&gt;\n\nПо умолчанию в него включены 12 основных ГОСТ-ов, по которым оформляется пояснительная записка. Чтобы добавить свои источники, введите их через перевод строки в одном сообщении:', 'sources'),</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="119" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="C36" s="1" t="str">
+        <f t="shared" si="8"/>
+        <v>'term_1': '',</v>
+      </c>
+      <c r="D36" s="1" t="str">
+        <f t="shared" si="9"/>
+        <v>('&lt;b&gt;Наконец заполним одно из приложений в качестве примера.&lt;/b&gt;\n\nНе забудьте дозаполнить таблицы, которые генерируются по умолчанию в приложениях. Вы сможете после сохранения документа в формате .docx.\n\nВведите любой технический термин из текста вашей пояснительной записки:', 'term_1'),</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A37" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="B36" s="1" t="s">
+      <c r="B37" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="C36" s="1" t="str">
-        <f t="shared" si="6"/>
-        <v>'term_1': '',</v>
-      </c>
-      <c r="D36" s="1" t="str">
-        <f t="shared" si="7"/>
-        <v>('&lt;b&gt;Наконец заполним одно из приложений в качестве примера.&lt;/b&gt;\n\nНе забудьте дозаполнить таблицы, которые генерируются по умолчанию в приложениях. Вы сможете после сохранения документа в формате .docx.\n\nВведите любой технический термин из текста вашей пояснительной записки:', 'term_1'),</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" ht="68" x14ac:dyDescent="0.2">
-      <c r="A37" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>140</v>
-      </c>
       <c r="C37" s="1" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>'definition_1': '',</v>
       </c>
       <c r="D37" s="1" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>('Введите определение введенного выше термина:', 'definition_1'),</v>
       </c>
     </row>

</xml_diff>